<commit_message>
fixed S2 data prep
</commit_message>
<xml_diff>
--- a/Analyses/S2_softRobots/t2_CAMs/outputs/01_dataPreperation/final/networkIndicators_post_final.xlsx
+++ b/Analyses/S2_softRobots/t2_CAMs/outputs/01_dataPreperation/final/networkIndicators_post_final.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="692">
   <si>
     <t>CAM_ID</t>
   </si>
@@ -792,6 +792,654 @@
   </si>
   <si>
     <t>225</t>
+  </si>
+  <si>
+    <t>d45664a2-fc8f-4623-bf4e-f6c82a573f61</t>
+  </si>
+  <si>
+    <t>6fc79693-7f8a-4b8e-9d16-54481d6614ff</t>
+  </si>
+  <si>
+    <t>6c2f1cf1-e16a-4d1c-893b-14600b3b6847</t>
+  </si>
+  <si>
+    <t>4ece5897-1e1f-4fe7-9686-91cfeba1be89</t>
+  </si>
+  <si>
+    <t>e236ce4a-8bd5-4236-915c-f6c51fc09a85</t>
+  </si>
+  <si>
+    <t>17a40280-d565-4ec7-b02a-565a0e25cb0d</t>
+  </si>
+  <si>
+    <t>f064826c-748c-4f53-9b49-b878ee1e8762</t>
+  </si>
+  <si>
+    <t>2be0e67b-ec5d-4448-8cb7-9325c223eb78</t>
+  </si>
+  <si>
+    <t>1a106295-c52d-448c-87ee-900913fa3118</t>
+  </si>
+  <si>
+    <t>f7c0ffb8-8e24-4f0e-91e6-bab4aacc25a5</t>
+  </si>
+  <si>
+    <t>0eced62b-80f1-4103-8d41-4cfc1429b741</t>
+  </si>
+  <si>
+    <t>c8a06638-b13e-4d76-891e-dedf2adc088b</t>
+  </si>
+  <si>
+    <t>91598ac7-8fd5-4d3d-a9c2-6d204d51596b</t>
+  </si>
+  <si>
+    <t>f5a16aa2-0177-4e56-9bcf-3baa1acba62e</t>
+  </si>
+  <si>
+    <t>30e20ee6-baf8-4bec-a8af-73a067bc6a28</t>
+  </si>
+  <si>
+    <t>cef58ca6-37aa-46f9-bdc1-e4029eb118f6</t>
+  </si>
+  <si>
+    <t>da40f057-a03b-42e0-8690-6fba7dd1a60f</t>
+  </si>
+  <si>
+    <t>eeee6ecf-ccfa-4d7f-9762-35373dd6c67a</t>
+  </si>
+  <si>
+    <t>85d26b27-16ea-4139-b2b6-d3b6310ee85b</t>
+  </si>
+  <si>
+    <t>256fa744-589c-441c-9270-0bfb8d4b4f9d</t>
+  </si>
+  <si>
+    <t>b4442081-ddc8-4bcb-9861-d6a417feff71</t>
+  </si>
+  <si>
+    <t>2f7a18af-ee68-4200-a9bd-768a6ea3b993</t>
+  </si>
+  <si>
+    <t>eb04f93e-2db7-43af-a5cc-f4fd53261e52</t>
+  </si>
+  <si>
+    <t>7cbe81ff-cffb-4a0d-ba55-929fb844e5f8</t>
+  </si>
+  <si>
+    <t>5db89e68-ae18-43c5-9907-d8ef139fbde7</t>
+  </si>
+  <si>
+    <t>e1add64c-9388-4430-aea3-50af1c5b2466</t>
+  </si>
+  <si>
+    <t>44ae2972-4a4f-4b25-9d6d-dff38f4e5425</t>
+  </si>
+  <si>
+    <t>a8232c86-7227-45b8-aed4-bad62adce95a</t>
+  </si>
+  <si>
+    <t>48d7cb36-6296-419e-bcaf-7f6c9490c9f6</t>
+  </si>
+  <si>
+    <t>ea9a7aef-d2d9-4c7d-933d-fcfb10e32536</t>
+  </si>
+  <si>
+    <t>7d287bdd-b024-4edf-805d-e6bdccc8bcd0</t>
+  </si>
+  <si>
+    <t>f9dd4433-7a2d-4e79-9de3-294f4c0f00ac</t>
+  </si>
+  <si>
+    <t>463f299d-2c26-468b-9bd1-3be9e763a087</t>
+  </si>
+  <si>
+    <t>e0fb180d-d3c1-4c13-9b0e-aff3a6bb9e01</t>
+  </si>
+  <si>
+    <t>4e342ef6-788f-47a0-ad8a-dad334a81b5f</t>
+  </si>
+  <si>
+    <t>2ed39bbe-bca0-41f2-be1d-4ccbecff78c3</t>
+  </si>
+  <si>
+    <t>41ccf4ef-c536-4f5e-aa8e-292032f35d62</t>
+  </si>
+  <si>
+    <t>8266b0f2-38e4-409e-a2e8-2bfd10924aec</t>
+  </si>
+  <si>
+    <t>5ba60b17-751d-450e-9566-f2955d2433cd</t>
+  </si>
+  <si>
+    <t>caa32b83-d911-4d59-ab0a-dba5407dc9f1</t>
+  </si>
+  <si>
+    <t>8707353a-d1a2-4197-9a50-7e161f4f127d</t>
+  </si>
+  <si>
+    <t>777642fe-649e-4f5b-b4c5-4317fe5f277b</t>
+  </si>
+  <si>
+    <t>27a66727-7f19-4a5c-a827-4e30a0a93981</t>
+  </si>
+  <si>
+    <t>a90498e2-9108-4c54-acf0-5c44fac4cc13</t>
+  </si>
+  <si>
+    <t>353a2754-a2cc-4dcf-a1cd-725ed219b0eb</t>
+  </si>
+  <si>
+    <t>d5ab7d2c-c598-467a-850f-2f25a6c55fba</t>
+  </si>
+  <si>
+    <t>2445685a-c6da-4fb3-be12-203bf7f7a9e5</t>
+  </si>
+  <si>
+    <t>1a84518d-a0b5-4bd5-9453-f7b96b68f7a7</t>
+  </si>
+  <si>
+    <t>091de011-c6dd-4ca7-94f7-c13056fcdb9d</t>
+  </si>
+  <si>
+    <t>cae4bae1-d581-4261-bb7a-ba1e05b7f837</t>
+  </si>
+  <si>
+    <t>599d19a2-088a-4836-adcd-8183ebe43ede</t>
+  </si>
+  <si>
+    <t>cc7fe4f6-5d53-41f9-b521-e9f42a05600b</t>
+  </si>
+  <si>
+    <t>2ce89ea6-24c5-4dab-88bc-830e11c4519e</t>
+  </si>
+  <si>
+    <t>70e4c579-a731-4c64-abb1-b4695ac3665a</t>
+  </si>
+  <si>
+    <t>382337d8-4501-40e3-8731-a294f1f89832</t>
+  </si>
+  <si>
+    <t>06833db4-f679-481e-a886-120d5ebaaba8</t>
+  </si>
+  <si>
+    <t>2db177d4-28b3-4736-9646-e701b2d42e24</t>
+  </si>
+  <si>
+    <t>8345107a-6a93-46e4-897f-a45e35e5cc33</t>
+  </si>
+  <si>
+    <t>8c149b8d-9463-480b-b1d0-3a0dfa63c99a</t>
+  </si>
+  <si>
+    <t>9c89cd29-5028-44b1-a98b-5a4a4c87a5ea</t>
+  </si>
+  <si>
+    <t>5353f2c7-ca4c-4f7d-9c9d-d11d44da5777</t>
+  </si>
+  <si>
+    <t>904985db-9f35-4d24-9c94-e091c4dde25a</t>
+  </si>
+  <si>
+    <t>50f47fed-c265-404e-a2df-e73ff0b9df87</t>
+  </si>
+  <si>
+    <t>43c2dfbc-54f9-44da-9d0d-295494e76b99</t>
+  </si>
+  <si>
+    <t>02dc8eb4-5308-4282-8aa0-e946e0fd9668</t>
+  </si>
+  <si>
+    <t>2b2ce9e7-480f-4dd1-a3f0-141d2d77369c</t>
+  </si>
+  <si>
+    <t>2ca2598d-d5b0-41f6-b494-4f2c6c60f3a5</t>
+  </si>
+  <si>
+    <t>7df9cac3-cec8-4199-b995-bd78231559c7</t>
+  </si>
+  <si>
+    <t>8ec971d2-7259-46a4-85ca-ae4f227ada5f</t>
+  </si>
+  <si>
+    <t>285a8bb6-a93b-4270-8cb5-29121336b0ee</t>
+  </si>
+  <si>
+    <t>f479bd76-85c1-4a66-bfbf-26f8be98f5c6</t>
+  </si>
+  <si>
+    <t>2e35137a-3321-4b53-b679-6efea72dfd4f</t>
+  </si>
+  <si>
+    <t>5a268fa4-fe21-4dd8-a37a-7fde53fe8c35</t>
+  </si>
+  <si>
+    <t>d620721a-16a1-4238-8f2d-c2fc124bbe7b</t>
+  </si>
+  <si>
+    <t>05e47d13-d2a0-433c-befc-18f2f6e4043e</t>
+  </si>
+  <si>
+    <t>25de95ab-ee78-4250-ae8e-dc21f9f78df7</t>
+  </si>
+  <si>
+    <t>e569238c-d670-40ce-aac9-04ed91b3a7fb</t>
+  </si>
+  <si>
+    <t>14fda0f2-2bcb-46d2-9c9e-79d74d33bcff</t>
+  </si>
+  <si>
+    <t>350ee43f-535b-43f3-94f3-350de1b26d37</t>
+  </si>
+  <si>
+    <t>1b96e230-f35d-47f6-b6c9-802d8accec33</t>
+  </si>
+  <si>
+    <t>6dc0c9bc-92ad-4fbb-8450-e2d6db8eaf5c</t>
+  </si>
+  <si>
+    <t>443d63c6-beda-47f0-ad96-3f7c91a37e61</t>
+  </si>
+  <si>
+    <t>9d9ebddf-4a0a-4f1f-8e4d-a2b40ec24b28</t>
+  </si>
+  <si>
+    <t>e26ecb6c-b399-4ed4-b40f-819a4cd7f710</t>
+  </si>
+  <si>
+    <t>0ae9dfe5-de0f-4c9a-98e1-779bc13b0953</t>
+  </si>
+  <si>
+    <t>b263d46c-33d0-420a-b454-4679f023e272</t>
+  </si>
+  <si>
+    <t>f1fe50c3-e6b4-4995-a218-a0b29ca816c9</t>
+  </si>
+  <si>
+    <t>8ba5b5c3-cca9-4dc1-8299-f9d5a8d0f198</t>
+  </si>
+  <si>
+    <t>9bf47935-450a-41f5-942c-69d8913df831</t>
+  </si>
+  <si>
+    <t>b7b62b80-acaf-47d7-9bdd-8dd1b7f3bee9</t>
+  </si>
+  <si>
+    <t>cb7103ee-14f2-4334-882a-768c5d51b8a7</t>
+  </si>
+  <si>
+    <t>119c6bf0-53b0-498d-8409-af66c65b81ad</t>
+  </si>
+  <si>
+    <t>c29c5832-f514-40cb-b69b-6f0bae1e786a</t>
+  </si>
+  <si>
+    <t>f3737731-879e-4ecb-b7e1-2f2ec5694c8d</t>
+  </si>
+  <si>
+    <t>f19fa2af-34b4-4033-8d15-2063fe2f355b</t>
+  </si>
+  <si>
+    <t>c7a79bf3-1d7e-414a-8639-b86adc2fe9f4</t>
+  </si>
+  <si>
+    <t>92060116-caec-4089-975c-1baeefc0ffbb</t>
+  </si>
+  <si>
+    <t>d5ef6768-5cd5-43f8-a836-0b62479e61e9</t>
+  </si>
+  <si>
+    <t>4b2cbe3a-9f8d-4fc9-920e-064c877e4c29</t>
+  </si>
+  <si>
+    <t>c0f85d2d-bccf-41e9-a7f3-b4f10663af4c</t>
+  </si>
+  <si>
+    <t>b7115bd6-d8ca-47a6-9d56-7a4256244f0f</t>
+  </si>
+  <si>
+    <t>661eec8b-7dda-4b22-9407-0075ca82bfe8</t>
+  </si>
+  <si>
+    <t>d4319aff-6a99-4385-affc-23698a666c65</t>
+  </si>
+  <si>
+    <t>e81ee96f-9ad5-4925-9e2c-cce33ef9bb26</t>
+  </si>
+  <si>
+    <t>788f6a86-b45e-40c4-ba19-3957c5dbd5d6</t>
+  </si>
+  <si>
+    <t>2f342c39-d1aa-4b2a-805a-0c45f3ee3ea5</t>
+  </si>
+  <si>
+    <t>c392b2bf-f22c-41bb-a005-2c3c47e98a55</t>
+  </si>
+  <si>
+    <t>46325093-6fb6-4854-a3c2-3121e5467a5a</t>
+  </si>
+  <si>
+    <t>f875c5f0-da50-4cbc-a51a-51826ba3939f</t>
+  </si>
+  <si>
+    <t>372089fd-a4b7-4819-a01b-7613a516aed3</t>
+  </si>
+  <si>
+    <t>4225aced-b8fc-4526-858e-e35c2bab452c</t>
+  </si>
+  <si>
+    <t>e0bc6ad0-6927-49a0-affd-55d8719edc88</t>
+  </si>
+  <si>
+    <t>88d136b5-761b-4d04-9261-a722322252bf</t>
+  </si>
+  <si>
+    <t>31a082ae-ea60-4afe-be12-27e007e4d8ef</t>
+  </si>
+  <si>
+    <t>8b64667f-efa2-481e-8ceb-cf37447f386f</t>
+  </si>
+  <si>
+    <t>7da97508-bba6-403b-b52d-27a6a8fb50f4</t>
+  </si>
+  <si>
+    <t>fc8155dd-2cd4-4853-8f72-a8b5c94acf9b</t>
+  </si>
+  <si>
+    <t>0d75e7af-f4fe-49b7-96b7-a1ec2c5df630</t>
+  </si>
+  <si>
+    <t>6f451ab9-87a3-4c66-97ef-747369dc423a</t>
+  </si>
+  <si>
+    <t>d6668905-c1e0-480a-a2e6-67b8f781a8f9</t>
+  </si>
+  <si>
+    <t>f181f5f9-604b-477f-9495-98c72b166356</t>
+  </si>
+  <si>
+    <t>409a5621-a860-4d22-8c80-1a892d8a985f</t>
+  </si>
+  <si>
+    <t>24c85861-bf8d-485b-848f-478a9fc3c33b</t>
+  </si>
+  <si>
+    <t>199097df-b3ea-40d2-9ac5-2b2a8c904033</t>
+  </si>
+  <si>
+    <t>0120ecba-5e43-4098-8d1e-12bf1ceaa771</t>
+  </si>
+  <si>
+    <t>a1b238c7-507f-41e7-864b-98879feafd4b</t>
+  </si>
+  <si>
+    <t>287e17fd-2803-4c94-9957-74d5916e39db</t>
+  </si>
+  <si>
+    <t>a706a0c5-1e5e-4caf-bb75-2cbf2e5c8174</t>
+  </si>
+  <si>
+    <t>2fdc5751-57f8-4925-a044-5587a26a31e4</t>
+  </si>
+  <si>
+    <t>83adecc7-c698-4781-a2a6-195f13cfd11f</t>
+  </si>
+  <si>
+    <t>d922a3c6-96c9-42f6-b86f-7085ed5baa4c</t>
+  </si>
+  <si>
+    <t>21e4b4ff-c402-482e-9670-4409b21144d4</t>
+  </si>
+  <si>
+    <t>403de1a7-3224-4069-980c-4c3a73d1d996</t>
+  </si>
+  <si>
+    <t>652b168e-01c6-4164-b913-0f070009feac</t>
+  </si>
+  <si>
+    <t>6fe9a16a-57d4-4100-95e8-4074efc73762</t>
+  </si>
+  <si>
+    <t>38ee6df5-6eac-4dee-a120-f7010eb51705</t>
+  </si>
+  <si>
+    <t>cdfb1abc-9ec9-416a-8cab-788a383b80ed</t>
+  </si>
+  <si>
+    <t>fed27d39-046c-474a-a0de-4f2dd50fd7ee</t>
+  </si>
+  <si>
+    <t>5d1a7d4a-9a66-4c29-9279-31bb23cd9c76</t>
+  </si>
+  <si>
+    <t>caf22493-a6fe-4694-ab0e-13474760caba</t>
+  </si>
+  <si>
+    <t>5e8da209-c6d9-4b34-a15e-3ed50573ab70</t>
+  </si>
+  <si>
+    <t>9706c210-2b4a-4933-96a0-cfca889b7f55</t>
+  </si>
+  <si>
+    <t>3ffea022-3e79-4b6c-b3e7-b0bfa541bf56</t>
+  </si>
+  <si>
+    <t>dc7f6055-bc76-40b4-8827-5fc0873d0af3</t>
+  </si>
+  <si>
+    <t>595c3fcc-3866-483b-8233-3bde0dc093de</t>
+  </si>
+  <si>
+    <t>4a8a5182-6515-48cb-b861-c3933c0faa8f</t>
+  </si>
+  <si>
+    <t>d3a9c21a-9b49-4d7c-bf72-edc35a31372f</t>
+  </si>
+  <si>
+    <t>8e51dcc8-f903-41e3-b7ae-2a2296fe3151</t>
+  </si>
+  <si>
+    <t>2bc204c6-27eb-43b3-af0a-a14cccdced09</t>
+  </si>
+  <si>
+    <t>f51f75fc-852a-4309-84e6-ae2289855c97</t>
+  </si>
+  <si>
+    <t>ec1bcbba-b09a-4204-bb25-80e30a0149a6</t>
+  </si>
+  <si>
+    <t>c827cbaa-f19f-4cf9-86ed-caab95f6249e</t>
+  </si>
+  <si>
+    <t>133a5382-04b2-4a8e-9f77-cf8857cfdae5</t>
+  </si>
+  <si>
+    <t>6330506a-e434-496c-bfff-d2499d93d75a</t>
+  </si>
+  <si>
+    <t>d17d8d55-ddac-4bb0-bcd3-40cbcb787fe9</t>
+  </si>
+  <si>
+    <t>adeb5384-7db9-4dbc-83ef-8623b7c546f3</t>
+  </si>
+  <si>
+    <t>61aaa381-5a19-4b24-b38b-2cfa7b23214b</t>
+  </si>
+  <si>
+    <t>19651a55-eede-4bcc-9b61-53a60b8f8867</t>
+  </si>
+  <si>
+    <t>62600d72-760f-470d-949a-986204c8162d</t>
+  </si>
+  <si>
+    <t>516db3b3-faed-4398-9adc-e7d3262837f4</t>
+  </si>
+  <si>
+    <t>82aa169c-e55c-4251-b189-5ed9e87cc8a4</t>
+  </si>
+  <si>
+    <t>875815c8-5264-413b-af44-ec5cc33e0b58</t>
+  </si>
+  <si>
+    <t>de3d10a5-41f6-4ed1-bb53-9f4267f22f5c</t>
+  </si>
+  <si>
+    <t>abe2e6ef-e65b-4958-9d30-7d8bf71e9348</t>
+  </si>
+  <si>
+    <t>1c769611-a9db-49b8-87b3-17fd59b717aa</t>
+  </si>
+  <si>
+    <t>d1293612-d08d-468f-87fb-daed63b517ed</t>
+  </si>
+  <si>
+    <t>13eb8adc-d55b-44ae-8fd4-9ff8056d727c</t>
+  </si>
+  <si>
+    <t>9b401cc5-ff2d-49a9-af03-af7014152a44</t>
+  </si>
+  <si>
+    <t>7e7c2213-3385-451d-84bb-3094ddd197a4</t>
+  </si>
+  <si>
+    <t>871cf0f6-89d6-454a-9f20-345137f6831c</t>
+  </si>
+  <si>
+    <t>7bf06044-f792-4703-a11d-01974859cce6</t>
+  </si>
+  <si>
+    <t>0c3017b6-164f-4a6a-b6f7-988331dd5b9b</t>
+  </si>
+  <si>
+    <t>43df7aff-d2aa-4761-b612-53a4390efc6b</t>
+  </si>
+  <si>
+    <t>4ca5f6a3-20cc-46aa-8ee5-1893d1592b0d</t>
+  </si>
+  <si>
+    <t>7e067bd1-09c4-4422-a6fa-291a7d33538b</t>
+  </si>
+  <si>
+    <t>6d267809-8427-4849-954a-8076ccfc1938</t>
+  </si>
+  <si>
+    <t>ab4cdc76-df43-4dfb-9fca-a815141e6b9c</t>
+  </si>
+  <si>
+    <t>70c94109-5514-4426-8f0f-f5b149f1fb51</t>
+  </si>
+  <si>
+    <t>4e3d961a-6288-41f5-8784-cb2ad20a93e7</t>
+  </si>
+  <si>
+    <t>248d70bc-a123-48dd-8e0f-981e51315526</t>
+  </si>
+  <si>
+    <t>ec191fe0-d1f9-4541-a8db-f216feb91c97</t>
+  </si>
+  <si>
+    <t>334b7ca1-32a4-4b6d-990e-5254b95dc9da</t>
+  </si>
+  <si>
+    <t>188ce7c2-cfb9-4c12-904f-aba1d0762a29</t>
+  </si>
+  <si>
+    <t>53048963-b319-44e5-92a8-6a7d0451d672</t>
+  </si>
+  <si>
+    <t>cc1b96bc-6512-45dd-8cb0-c711fa1ce1f7</t>
+  </si>
+  <si>
+    <t>af77986f-d119-47ab-b2c1-744d978b9905</t>
+  </si>
+  <si>
+    <t>ac4d0c1d-1129-45ec-b82e-99b8de1e0b46</t>
+  </si>
+  <si>
+    <t>a32586c3-9eef-4fac-aa13-5555057d6921</t>
+  </si>
+  <si>
+    <t>84202912-6234-4864-85cf-99a470dcb6bd</t>
+  </si>
+  <si>
+    <t>8886ccab-47f8-4c3a-b75c-3056b367cf00</t>
+  </si>
+  <si>
+    <t>673a3512-648e-475f-9f93-6518c33a49d5</t>
+  </si>
+  <si>
+    <t>95d5f60a-f397-467a-823c-be580f1eb850</t>
+  </si>
+  <si>
+    <t>a371bdb0-b463-4c73-8524-0dc5d519df9f</t>
+  </si>
+  <si>
+    <t>8a8699d1-f6fc-4708-9ddc-0d0a05d9a57a</t>
+  </si>
+  <si>
+    <t>65d3330c-33f7-4ca4-b2d3-e1d9678bdf2a</t>
+  </si>
+  <si>
+    <t>749a54ae-7c4e-494c-8998-0df4c880b48e</t>
+  </si>
+  <si>
+    <t>b46a3f85-272a-4fb1-a8c9-52bd1b1c5d5e</t>
+  </si>
+  <si>
+    <t>b66fb4ed-51c3-45dd-b6f5-a64ccb12003b</t>
+  </si>
+  <si>
+    <t>5ba92f91-c07e-47eb-9e06-7cf035d23072</t>
+  </si>
+  <si>
+    <t>e34e30fb-fd82-4197-9e0c-a7e4d64e18bc</t>
+  </si>
+  <si>
+    <t>8005126e-ab25-495b-8826-56cc7f3520b4</t>
+  </si>
+  <si>
+    <t>7f00077a-e532-4562-a571-43d3e2877715</t>
+  </si>
+  <si>
+    <t>0908490f-5979-4981-808f-6c2517d983b6</t>
+  </si>
+  <si>
+    <t>63ff4f0c-c090-435e-af21-747074124355</t>
+  </si>
+  <si>
+    <t>136497ab-676e-46a6-9d6d-8c00bf1c0c7c</t>
+  </si>
+  <si>
+    <t>d5b059ab-21d0-4681-bb3b-a70c65982f71</t>
+  </si>
+  <si>
+    <t>93968145-0a28-4263-ac64-4814d339fc56</t>
+  </si>
+  <si>
+    <t>696d9fb7-1b96-43df-b796-55a1cfaf3271</t>
+  </si>
+  <si>
+    <t>ed155092-2336-4ac3-8391-ef8ca80c2649</t>
+  </si>
+  <si>
+    <t>e9f941af-2243-49e2-9f89-dd3daf9b7f03</t>
+  </si>
+  <si>
+    <t>ea195ea3-bec2-46a7-99ee-5bdce4e78871</t>
+  </si>
+  <si>
+    <t>0d39e230-e0e6-4506-bb8b-9603b89b601c</t>
+  </si>
+  <si>
+    <t>11a237fd-68bb-4cc7-b7dc-97476d374037</t>
+  </si>
+  <si>
+    <t>68d530a8-abef-460c-80bc-90aa1dfcf7ce</t>
+  </si>
+  <si>
+    <t>61cef66b-35f0-4ca2-9b0a-7b3218df9b49</t>
+  </si>
+  <si>
+    <t>9199241d-cdbf-443e-9053-9e5ad8551802</t>
   </si>
   <si>
     <t>643cff9260890a3b38e3130d</t>
@@ -1633,7 +2281,7 @@
         <v>260</v>
       </c>
       <c r="C2" t="s">
-        <v>260</v>
+        <v>476</v>
       </c>
       <c r="D2" t="n">
         <v>0.17391304347826086</v>
@@ -1657,7 +2305,7 @@
         <v>0.6550570641479733</v>
       </c>
       <c r="K2" t="n">
-        <v>0.7423890598447438</v>
+        <v>0.7423890598447433</v>
       </c>
       <c r="L2" t="n">
         <v>2.375</v>
@@ -1762,7 +2410,7 @@
         <v>261</v>
       </c>
       <c r="C3" t="s">
-        <v>261</v>
+        <v>477</v>
       </c>
       <c r="D3" t="n">
         <v>0.2857142857142857</v>
@@ -1786,7 +2434,7 @@
         <v>0.5364891518737672</v>
       </c>
       <c r="K3" t="n">
-        <v>0.6280353788176075</v>
+        <v>0.6280353788176077</v>
       </c>
       <c r="L3" t="n">
         <v>1.4705882352941178</v>
@@ -1891,7 +2539,7 @@
         <v>262</v>
       </c>
       <c r="C4" t="s">
-        <v>262</v>
+        <v>478</v>
       </c>
       <c r="D4" t="n">
         <v>-0.6153846153846154</v>
@@ -1915,7 +2563,7 @@
         <v>0.38667929292929293</v>
       </c>
       <c r="K4" t="n">
-        <v>0.5414506112685875</v>
+        <v>0.5414506112685872</v>
       </c>
       <c r="L4" t="n">
         <v>5.5</v>
@@ -2020,7 +2668,7 @@
         <v>263</v>
       </c>
       <c r="C5" t="s">
-        <v>263</v>
+        <v>479</v>
       </c>
       <c r="D5" t="n">
         <v>0.375</v>
@@ -2044,7 +2692,7 @@
         <v>0.35174603174603175</v>
       </c>
       <c r="K5" t="n">
-        <v>0.7400106338867255</v>
+        <v>0.7400106338867257</v>
       </c>
       <c r="L5" t="n">
         <v>1.8</v>
@@ -2149,7 +2797,7 @@
         <v>264</v>
       </c>
       <c r="C6" t="s">
-        <v>264</v>
+        <v>480</v>
       </c>
       <c r="D6" t="n">
         <v>0.4</v>
@@ -2173,7 +2821,7 @@
         <v>0.6043956043956044</v>
       </c>
       <c r="K6" t="n">
-        <v>0.6192501947457051</v>
+        <v>0.6192501947457054</v>
       </c>
       <c r="L6" t="n">
         <v>1.0</v>
@@ -2278,7 +2926,7 @@
         <v>265</v>
       </c>
       <c r="C7" t="s">
-        <v>265</v>
+        <v>481</v>
       </c>
       <c r="D7" t="n">
         <v>0.8333333333333334</v>
@@ -2302,7 +2950,7 @@
         <v>0.6640576230492197</v>
       </c>
       <c r="K7" t="n">
-        <v>0.819615094884234</v>
+        <v>0.8196150948842338</v>
       </c>
       <c r="L7" t="n">
         <v>2.706896551724138</v>
@@ -2407,7 +3055,7 @@
         <v>266</v>
       </c>
       <c r="C8" t="s">
-        <v>266</v>
+        <v>482</v>
       </c>
       <c r="D8" t="n">
         <v>-0.05263157894736842</v>
@@ -2431,7 +3079,7 @@
         <v>0.555918663761801</v>
       </c>
       <c r="K8" t="n">
-        <v>0.6932295827470418</v>
+        <v>0.6932295827470416</v>
       </c>
       <c r="L8" t="n">
         <v>3.4722222222222223</v>
@@ -2536,7 +3184,7 @@
         <v>267</v>
       </c>
       <c r="C9" t="s">
-        <v>267</v>
+        <v>483</v>
       </c>
       <c r="D9" t="n">
         <v>0.11764705882352941</v>
@@ -2665,7 +3313,7 @@
         <v>268</v>
       </c>
       <c r="C10" t="s">
-        <v>268</v>
+        <v>484</v>
       </c>
       <c r="D10" t="n">
         <v>-0.25</v>
@@ -2689,7 +3337,7 @@
         <v>0.8091005291005292</v>
       </c>
       <c r="K10" t="n">
-        <v>0.7414111553854237</v>
+        <v>0.7414111553854236</v>
       </c>
       <c r="L10" t="n">
         <v>3.576</v>
@@ -2794,7 +3442,7 @@
         <v>269</v>
       </c>
       <c r="C11" t="s">
-        <v>269</v>
+        <v>485</v>
       </c>
       <c r="D11" t="n">
         <v>0.47058823529411764</v>
@@ -2818,7 +3466,7 @@
         <v>0.615625</v>
       </c>
       <c r="K11" t="n">
-        <v>0.7300163799033652</v>
+        <v>0.7300163799033653</v>
       </c>
       <c r="L11" t="n">
         <v>1.8181818181818181</v>
@@ -2923,7 +3571,7 @@
         <v>270</v>
       </c>
       <c r="C12" t="s">
-        <v>270</v>
+        <v>486</v>
       </c>
       <c r="D12" t="n">
         <v>0.23076923076923078</v>
@@ -2947,7 +3595,7 @@
         <v>0.41023929773929774</v>
       </c>
       <c r="K12" t="n">
-        <v>0.5729568581892689</v>
+        <v>0.5729568581892687</v>
       </c>
       <c r="L12" t="n">
         <v>2.731707317073171</v>
@@ -3052,7 +3700,7 @@
         <v>271</v>
       </c>
       <c r="C13" t="s">
-        <v>271</v>
+        <v>487</v>
       </c>
       <c r="D13" t="n">
         <v>-0.0625</v>
@@ -3076,7 +3724,7 @@
         <v>0.6273015873015872</v>
       </c>
       <c r="K13" t="n">
-        <v>0.7296017761127148</v>
+        <v>0.7296017761127144</v>
       </c>
       <c r="L13" t="n">
         <v>3.375</v>
@@ -3181,7 +3829,7 @@
         <v>272</v>
       </c>
       <c r="C14" t="s">
-        <v>272</v>
+        <v>488</v>
       </c>
       <c r="D14" t="n">
         <v>0.5</v>
@@ -3310,7 +3958,7 @@
         <v>273</v>
       </c>
       <c r="C15" t="s">
-        <v>273</v>
+        <v>489</v>
       </c>
       <c r="D15" t="n">
         <v>-0.5</v>
@@ -3334,7 +3982,7 @@
         <v>0.5733333333333334</v>
       </c>
       <c r="K15" t="n">
-        <v>0.720552640188315</v>
+        <v>0.7205526401883152</v>
       </c>
       <c r="L15" t="n">
         <v>2.303030303030303</v>
@@ -3439,7 +4087,7 @@
         <v>274</v>
       </c>
       <c r="C16" t="s">
-        <v>274</v>
+        <v>490</v>
       </c>
       <c r="D16" t="n">
         <v>1.0526315789473684</v>
@@ -3568,7 +4216,7 @@
         <v>275</v>
       </c>
       <c r="C17" t="s">
-        <v>275</v>
+        <v>491</v>
       </c>
       <c r="D17" t="n">
         <v>-0.09090909090909091</v>
@@ -3592,7 +4240,7 @@
         <v>0.6711111111111111</v>
       </c>
       <c r="K17" t="n">
-        <v>0.7291671489030338</v>
+        <v>0.7291671489030337</v>
       </c>
       <c r="L17" t="n">
         <v>3.0</v>
@@ -3697,7 +4345,7 @@
         <v>276</v>
       </c>
       <c r="C18" t="s">
-        <v>276</v>
+        <v>492</v>
       </c>
       <c r="D18" t="n">
         <v>-0.07142857142857142</v>
@@ -3826,7 +4474,7 @@
         <v>277</v>
       </c>
       <c r="C19" t="s">
-        <v>277</v>
+        <v>493</v>
       </c>
       <c r="D19" t="n">
         <v>-0.14285714285714285</v>
@@ -3850,7 +4498,7 @@
         <v>0.596646942800789</v>
       </c>
       <c r="K19" t="n">
-        <v>0.7217444379347056</v>
+        <v>0.7217444379347059</v>
       </c>
       <c r="L19" t="n">
         <v>1.434782608695652</v>
@@ -3955,7 +4603,7 @@
         <v>278</v>
       </c>
       <c r="C20" t="s">
-        <v>278</v>
+        <v>494</v>
       </c>
       <c r="D20" t="n">
         <v>0.15384615384615385</v>
@@ -3979,7 +4627,7 @@
         <v>0.6805555555555556</v>
       </c>
       <c r="K20" t="n">
-        <v>0.7503994041344021</v>
+        <v>0.7503994041344022</v>
       </c>
       <c r="L20" t="n">
         <v>1.5</v>
@@ -4084,7 +4732,7 @@
         <v>279</v>
       </c>
       <c r="C21" t="s">
-        <v>279</v>
+        <v>495</v>
       </c>
       <c r="D21" t="n">
         <v>-0.15384615384615385</v>
@@ -4213,7 +4861,7 @@
         <v>280</v>
       </c>
       <c r="C22" t="s">
-        <v>280</v>
+        <v>496</v>
       </c>
       <c r="D22" t="n">
         <v>0.2857142857142857</v>
@@ -4237,7 +4885,7 @@
         <v>0.6400394477317555</v>
       </c>
       <c r="K22" t="n">
-        <v>0.7085243743539139</v>
+        <v>0.7085243743539135</v>
       </c>
       <c r="L22" t="n">
         <v>1.5217391304347827</v>
@@ -4342,7 +4990,7 @@
         <v>281</v>
       </c>
       <c r="C23" t="s">
-        <v>281</v>
+        <v>497</v>
       </c>
       <c r="D23" t="n">
         <v>-0.375</v>
@@ -4471,7 +5119,7 @@
         <v>282</v>
       </c>
       <c r="C24" t="s">
-        <v>282</v>
+        <v>498</v>
       </c>
       <c r="D24" t="n">
         <v>0.0</v>
@@ -4495,7 +5143,7 @@
         <v>0.44635416666666666</v>
       </c>
       <c r="K24" t="n">
-        <v>0.6515685568801916</v>
+        <v>0.6515685568801917</v>
       </c>
       <c r="L24" t="n">
         <v>3.1587301587301586</v>
@@ -4600,7 +5248,7 @@
         <v>283</v>
       </c>
       <c r="C25" t="s">
-        <v>283</v>
+        <v>499</v>
       </c>
       <c r="D25" t="n">
         <v>-0.26666666666666666</v>
@@ -4624,7 +5272,7 @@
         <v>0.5149136577708007</v>
       </c>
       <c r="K25" t="n">
-        <v>0.7202576681922643</v>
+        <v>0.7202576681922632</v>
       </c>
       <c r="L25" t="n">
         <v>2.1372549019607843</v>
@@ -4729,7 +5377,7 @@
         <v>284</v>
       </c>
       <c r="C26" t="s">
-        <v>284</v>
+        <v>500</v>
       </c>
       <c r="D26" t="n">
         <v>0.5833333333333334</v>
@@ -4858,7 +5506,7 @@
         <v>285</v>
       </c>
       <c r="C27" t="s">
-        <v>285</v>
+        <v>501</v>
       </c>
       <c r="D27" t="n">
         <v>0.4838709677419355</v>
@@ -4882,7 +5530,7 @@
         <v>0.633256704980843</v>
       </c>
       <c r="K27" t="n">
-        <v>0.7808668713731206</v>
+        <v>0.7808668713731202</v>
       </c>
       <c r="L27" t="n">
         <v>1.6</v>
@@ -4987,7 +5635,7 @@
         <v>286</v>
       </c>
       <c r="C28" t="s">
-        <v>286</v>
+        <v>502</v>
       </c>
       <c r="D28" t="n">
         <v>0.3333333333333333</v>
@@ -5011,7 +5659,7 @@
         <v>0.5514705882352942</v>
       </c>
       <c r="K28" t="n">
-        <v>0.7020627893552873</v>
+        <v>0.7020627893552882</v>
       </c>
       <c r="L28" t="n">
         <v>2.89010989010989</v>
@@ -5116,7 +5764,7 @@
         <v>287</v>
       </c>
       <c r="C29" t="s">
-        <v>287</v>
+        <v>503</v>
       </c>
       <c r="D29" t="n">
         <v>0.15384615384615385</v>
@@ -5245,7 +5893,7 @@
         <v>288</v>
       </c>
       <c r="C30" t="s">
-        <v>288</v>
+        <v>504</v>
       </c>
       <c r="D30" t="n">
         <v>-0.07692307692307693</v>
@@ -5374,7 +6022,7 @@
         <v>289</v>
       </c>
       <c r="C31" t="s">
-        <v>289</v>
+        <v>505</v>
       </c>
       <c r="D31" t="n">
         <v>0.5</v>
@@ -5398,7 +6046,7 @@
         <v>0.546031746031746</v>
       </c>
       <c r="K31" t="n">
-        <v>0.6770405955186133</v>
+        <v>0.677040595518613</v>
       </c>
       <c r="L31" t="n">
         <v>2.6</v>
@@ -5503,7 +6151,7 @@
         <v>290</v>
       </c>
       <c r="C32" t="s">
-        <v>290</v>
+        <v>506</v>
       </c>
       <c r="D32" t="n">
         <v>1.1538461538461537</v>
@@ -5527,7 +6175,7 @@
         <v>0.51010101010101</v>
       </c>
       <c r="K32" t="n">
-        <v>0.622152256849212</v>
+        <v>0.6221522568492123</v>
       </c>
       <c r="L32" t="n">
         <v>1.6538461538461537</v>
@@ -5632,7 +6280,7 @@
         <v>291</v>
       </c>
       <c r="C33" t="s">
-        <v>291</v>
+        <v>507</v>
       </c>
       <c r="D33" t="n">
         <v>0.17857142857142858</v>
@@ -5656,7 +6304,7 @@
         <v>0.606943125461644</v>
       </c>
       <c r="K33" t="n">
-        <v>0.7911123087038979</v>
+        <v>0.791112308703898</v>
       </c>
       <c r="L33" t="n">
         <v>2.1717171717171717</v>
@@ -5761,7 +6409,7 @@
         <v>292</v>
       </c>
       <c r="C34" t="s">
-        <v>292</v>
+        <v>508</v>
       </c>
       <c r="D34" t="n">
         <v>-2.2857142857142856</v>
@@ -5785,7 +6433,7 @@
         <v>0.33228139381985544</v>
       </c>
       <c r="K34" t="n">
-        <v>0.5811148380473609</v>
+        <v>0.5811148380473606</v>
       </c>
       <c r="L34" t="n">
         <v>6.901639344262295</v>
@@ -5890,7 +6538,7 @@
         <v>293</v>
       </c>
       <c r="C35" t="s">
-        <v>293</v>
+        <v>509</v>
       </c>
       <c r="D35" t="n">
         <v>0.17391304347826086</v>
@@ -5914,7 +6562,7 @@
         <v>0.6302636757182212</v>
       </c>
       <c r="K35" t="n">
-        <v>0.7056051838996016</v>
+        <v>0.7056051838996015</v>
       </c>
       <c r="L35" t="n">
         <v>3.45</v>
@@ -6019,7 +6667,7 @@
         <v>294</v>
       </c>
       <c r="C36" t="s">
-        <v>294</v>
+        <v>510</v>
       </c>
       <c r="D36" t="n">
         <v>0.25</v>
@@ -6043,7 +6691,7 @@
         <v>0.5707166179755971</v>
       </c>
       <c r="K36" t="n">
-        <v>0.770607464020738</v>
+        <v>0.770607464020739</v>
       </c>
       <c r="L36" t="n">
         <v>1.7878787878787878</v>
@@ -6148,7 +6796,7 @@
         <v>295</v>
       </c>
       <c r="C37" t="s">
-        <v>295</v>
+        <v>511</v>
       </c>
       <c r="D37" t="n">
         <v>-0.1111111111111111</v>
@@ -6172,7 +6820,7 @@
         <v>0.4991349480968858</v>
       </c>
       <c r="K37" t="n">
-        <v>0.6972540736554401</v>
+        <v>0.6972540736554399</v>
       </c>
       <c r="L37" t="n">
         <v>1.9230769230769231</v>
@@ -6277,7 +6925,7 @@
         <v>296</v>
       </c>
       <c r="C38" t="s">
-        <v>296</v>
+        <v>512</v>
       </c>
       <c r="D38" t="n">
         <v>0.2</v>
@@ -6301,7 +6949,7 @@
         <v>0.595679012345679</v>
       </c>
       <c r="K38" t="n">
-        <v>0.6536855299290221</v>
+        <v>0.6536855299290218</v>
       </c>
       <c r="L38" t="n">
         <v>1.3333333333333333</v>
@@ -6406,7 +7054,7 @@
         <v>297</v>
       </c>
       <c r="C39" t="s">
-        <v>297</v>
+        <v>513</v>
       </c>
       <c r="D39" t="n">
         <v>-0.125</v>
@@ -6430,7 +7078,7 @@
         <v>0.6279365079365079</v>
       </c>
       <c r="K39" t="n">
-        <v>0.6750867163585547</v>
+        <v>0.6750867163585549</v>
       </c>
       <c r="L39" t="n">
         <v>3.8625</v>
@@ -6535,7 +7183,7 @@
         <v>298</v>
       </c>
       <c r="C40" t="s">
-        <v>298</v>
+        <v>514</v>
       </c>
       <c r="D40" t="n">
         <v>-0.26666666666666666</v>
@@ -6559,7 +7207,7 @@
         <v>0.6043956043956044</v>
       </c>
       <c r="K40" t="n">
-        <v>0.6192501947457052</v>
+        <v>0.6192501947457051</v>
       </c>
       <c r="L40" t="n">
         <v>2.875</v>
@@ -6664,7 +7312,7 @@
         <v>299</v>
       </c>
       <c r="C41" t="s">
-        <v>299</v>
+        <v>515</v>
       </c>
       <c r="D41" t="n">
         <v>-0.038461538461538464</v>
@@ -6688,7 +7336,7 @@
         <v>0.6056</v>
       </c>
       <c r="K41" t="n">
-        <v>0.7263578664227311</v>
+        <v>0.7263578664227305</v>
       </c>
       <c r="L41" t="n">
         <v>1.8409090909090908</v>
@@ -6793,7 +7441,7 @@
         <v>300</v>
       </c>
       <c r="C42" t="s">
-        <v>300</v>
+        <v>516</v>
       </c>
       <c r="D42" t="n">
         <v>0.25</v>
@@ -6817,7 +7465,7 @@
         <v>0.6429752066115703</v>
       </c>
       <c r="K42" t="n">
-        <v>0.7355499095234123</v>
+        <v>0.7355499095234124</v>
       </c>
       <c r="L42" t="n">
         <v>2.3333333333333335</v>
@@ -6922,7 +7570,7 @@
         <v>301</v>
       </c>
       <c r="C43" t="s">
-        <v>301</v>
+        <v>517</v>
       </c>
       <c r="D43" t="n">
         <v>0.25</v>
@@ -6946,7 +7594,7 @@
         <v>0.14380165289256197</v>
       </c>
       <c r="K43" t="n">
-        <v>0.34984261957130636</v>
+        <v>0.3498426195713069</v>
       </c>
       <c r="L43" t="n">
         <v>3.809090909090909</v>
@@ -7051,7 +7699,7 @@
         <v>302</v>
       </c>
       <c r="C44" t="s">
-        <v>302</v>
+        <v>518</v>
       </c>
       <c r="D44" t="n">
         <v>-0.5384615384615384</v>
@@ -7180,7 +7828,7 @@
         <v>303</v>
       </c>
       <c r="C45" t="s">
-        <v>303</v>
+        <v>519</v>
       </c>
       <c r="D45" t="n">
         <v>0.21428571428571427</v>
@@ -7204,7 +7852,7 @@
         <v>0.6370808678500987</v>
       </c>
       <c r="K45" t="n">
-        <v>0.6621504322623792</v>
+        <v>0.6621504322623794</v>
       </c>
       <c r="L45" t="n">
         <v>3.533333333333333</v>
@@ -7309,7 +7957,7 @@
         <v>304</v>
       </c>
       <c r="C46" t="s">
-        <v>304</v>
+        <v>520</v>
       </c>
       <c r="D46" t="n">
         <v>-0.07142857142857142</v>
@@ -7333,7 +7981,7 @@
         <v>0.6400394477317555</v>
       </c>
       <c r="K46" t="n">
-        <v>0.7085243743539135</v>
+        <v>0.7085243743539138</v>
       </c>
       <c r="L46" t="n">
         <v>1.8333333333333333</v>
@@ -7438,7 +8086,7 @@
         <v>305</v>
       </c>
       <c r="C47" t="s">
-        <v>305</v>
+        <v>521</v>
       </c>
       <c r="D47" t="n">
         <v>-0.3157894736842105</v>
@@ -7567,7 +8215,7 @@
         <v>306</v>
       </c>
       <c r="C48" t="s">
-        <v>306</v>
+        <v>522</v>
       </c>
       <c r="D48" t="n">
         <v>-0.35294117647058826</v>
@@ -7591,7 +8239,7 @@
         <v>0.5072916666666667</v>
       </c>
       <c r="K48" t="n">
-        <v>0.6410418120233882</v>
+        <v>0.6410418120233884</v>
       </c>
       <c r="L48" t="n">
         <v>3.051282051282051</v>
@@ -7696,7 +8344,7 @@
         <v>307</v>
       </c>
       <c r="C49" t="s">
-        <v>307</v>
+        <v>523</v>
       </c>
       <c r="D49" t="n">
         <v>0.2857142857142857</v>
@@ -7825,7 +8473,7 @@
         <v>308</v>
       </c>
       <c r="C50" t="s">
-        <v>308</v>
+        <v>524</v>
       </c>
       <c r="D50" t="n">
         <v>0.15384615384615385</v>
@@ -7849,7 +8497,7 @@
         <v>0.5795454545454546</v>
       </c>
       <c r="K50" t="n">
-        <v>0.58767512035357</v>
+        <v>0.5876751203535706</v>
       </c>
       <c r="L50" t="n">
         <v>2.7142857142857144</v>
@@ -7954,7 +8602,7 @@
         <v>309</v>
       </c>
       <c r="C51" t="s">
-        <v>309</v>
+        <v>525</v>
       </c>
       <c r="D51" t="n">
         <v>0.15384615384615385</v>
@@ -8083,7 +8731,7 @@
         <v>310</v>
       </c>
       <c r="C52" t="s">
-        <v>310</v>
+        <v>526</v>
       </c>
       <c r="D52" t="n">
         <v>0.0</v>
@@ -8107,7 +8755,7 @@
         <v>0.47672583826429976</v>
       </c>
       <c r="K52" t="n">
-        <v>0.5923475419384224</v>
+        <v>0.5923475419384225</v>
       </c>
       <c r="L52" t="n">
         <v>2.8679245283018866</v>
@@ -8212,7 +8860,7 @@
         <v>311</v>
       </c>
       <c r="C53" t="s">
-        <v>311</v>
+        <v>527</v>
       </c>
       <c r="D53" t="n">
         <v>0.24</v>
@@ -8341,7 +8989,7 @@
         <v>312</v>
       </c>
       <c r="C54" t="s">
-        <v>312</v>
+        <v>528</v>
       </c>
       <c r="D54" t="n">
         <v>0.8461538461538461</v>
@@ -8365,7 +9013,7 @@
         <v>0.6805555555555556</v>
       </c>
       <c r="K54" t="n">
-        <v>0.7503994041344023</v>
+        <v>0.7503994041344021</v>
       </c>
       <c r="L54" t="n">
         <v>2.0833333333333335</v>
@@ -8470,7 +9118,7 @@
         <v>313</v>
       </c>
       <c r="C55" t="s">
-        <v>313</v>
+        <v>529</v>
       </c>
       <c r="D55" t="n">
         <v>0.08333333333333333</v>
@@ -8494,7 +9142,7 @@
         <v>0.17851239669421487</v>
       </c>
       <c r="K55" t="n">
-        <v>0.5034267966167374</v>
+        <v>0.503426796616737</v>
       </c>
       <c r="L55" t="n">
         <v>3.185185185185185</v>
@@ -8599,7 +9247,7 @@
         <v>314</v>
       </c>
       <c r="C56" t="s">
-        <v>314</v>
+        <v>530</v>
       </c>
       <c r="D56" t="n">
         <v>-0.18181818181818182</v>
@@ -8728,7 +9376,7 @@
         <v>315</v>
       </c>
       <c r="C57" t="s">
-        <v>315</v>
+        <v>531</v>
       </c>
       <c r="D57" t="n">
         <v>0.2</v>
@@ -8752,7 +9400,7 @@
         <v>0.3371271585557299</v>
       </c>
       <c r="K57" t="n">
-        <v>0.646182340393027</v>
+        <v>0.6461823403930269</v>
       </c>
       <c r="L57" t="n">
         <v>2.2954545454545454</v>
@@ -8857,7 +9505,7 @@
         <v>316</v>
       </c>
       <c r="C58" t="s">
-        <v>316</v>
+        <v>532</v>
       </c>
       <c r="D58" t="n">
         <v>0.2857142857142857</v>
@@ -8881,7 +9529,7 @@
         <v>0.5601577909270217</v>
       </c>
       <c r="K58" t="n">
-        <v>0.6517448742559838</v>
+        <v>0.651744874255984</v>
       </c>
       <c r="L58" t="n">
         <v>2.1025641025641026</v>
@@ -8986,7 +9634,7 @@
         <v>317</v>
       </c>
       <c r="C59" t="s">
-        <v>317</v>
+        <v>533</v>
       </c>
       <c r="D59" t="n">
         <v>-0.18181818181818182</v>
@@ -9115,7 +9763,7 @@
         <v>318</v>
       </c>
       <c r="C60" t="s">
-        <v>318</v>
+        <v>534</v>
       </c>
       <c r="D60" t="n">
         <v>-0.21428571428571427</v>
@@ -9244,7 +9892,7 @@
         <v>319</v>
       </c>
       <c r="C61" t="s">
-        <v>319</v>
+        <v>535</v>
       </c>
       <c r="D61" t="n">
         <v>0.125</v>
@@ -9373,7 +10021,7 @@
         <v>320</v>
       </c>
       <c r="C62" t="s">
-        <v>320</v>
+        <v>536</v>
       </c>
       <c r="D62" t="n">
         <v>0.3125</v>
@@ -9502,7 +10150,7 @@
         <v>321</v>
       </c>
       <c r="C63" t="s">
-        <v>321</v>
+        <v>537</v>
       </c>
       <c r="D63" t="n">
         <v>-0.06666666666666667</v>
@@ -9526,7 +10174,7 @@
         <v>0.542386185243328</v>
       </c>
       <c r="K63" t="n">
-        <v>0.6797318422492198</v>
+        <v>0.6797318422492199</v>
       </c>
       <c r="L63" t="n">
         <v>1.82</v>
@@ -9631,7 +10279,7 @@
         <v>322</v>
       </c>
       <c r="C64" t="s">
-        <v>322</v>
+        <v>538</v>
       </c>
       <c r="D64" t="n">
         <v>-0.25</v>
@@ -9655,7 +10303,7 @@
         <v>0.34201058201058204</v>
       </c>
       <c r="K64" t="n">
-        <v>0.5581775385070361</v>
+        <v>0.5581775385070359</v>
       </c>
       <c r="L64" t="n">
         <v>1.9811320754716981</v>
@@ -9760,7 +10408,7 @@
         <v>323</v>
       </c>
       <c r="C65" t="s">
-        <v>323</v>
+        <v>539</v>
       </c>
       <c r="D65" t="n">
         <v>-0.23076923076923078</v>
@@ -9784,7 +10432,7 @@
         <v>0.6805555555555556</v>
       </c>
       <c r="K65" t="n">
-        <v>0.7503994041344022</v>
+        <v>0.7503994041344021</v>
       </c>
       <c r="L65" t="n">
         <v>1.9166666666666667</v>
@@ -9889,7 +10537,7 @@
         <v>324</v>
       </c>
       <c r="C66" t="s">
-        <v>324</v>
+        <v>540</v>
       </c>
       <c r="D66" t="n">
         <v>0.6153846153846154</v>
@@ -10018,7 +10666,7 @@
         <v>325</v>
       </c>
       <c r="C67" t="s">
-        <v>325</v>
+        <v>541</v>
       </c>
       <c r="D67" t="n">
         <v>0.5</v>
@@ -10147,7 +10795,7 @@
         <v>326</v>
       </c>
       <c r="C68" t="s">
-        <v>326</v>
+        <v>542</v>
       </c>
       <c r="D68" t="n">
         <v>0.23529411764705882</v>
@@ -10171,7 +10819,7 @@
         <v>0.6229166666666667</v>
       </c>
       <c r="K68" t="n">
-        <v>0.6444444444444447</v>
+        <v>0.6444444444444446</v>
       </c>
       <c r="L68" t="n">
         <v>2.066666666666667</v>
@@ -10276,7 +10924,7 @@
         <v>327</v>
       </c>
       <c r="C69" t="s">
-        <v>327</v>
+        <v>543</v>
       </c>
       <c r="D69" t="n">
         <v>0.4375</v>
@@ -10405,7 +11053,7 @@
         <v>328</v>
       </c>
       <c r="C70" t="s">
-        <v>328</v>
+        <v>544</v>
       </c>
       <c r="D70" t="n">
         <v>0.0</v>
@@ -10429,7 +11077,7 @@
         <v>0.6088888888888889</v>
       </c>
       <c r="K70" t="n">
-        <v>0.6533878071413058</v>
+        <v>0.6533878071413061</v>
       </c>
       <c r="L70" t="n">
         <v>1.1666666666666667</v>
@@ -10534,7 +11182,7 @@
         <v>329</v>
       </c>
       <c r="C71" t="s">
-        <v>329</v>
+        <v>545</v>
       </c>
       <c r="D71" t="n">
         <v>-0.06666666666666667</v>
@@ -10558,7 +11206,7 @@
         <v>0.5372841444270016</v>
       </c>
       <c r="K71" t="n">
-        <v>0.6716815734420242</v>
+        <v>0.6716815734420243</v>
       </c>
       <c r="L71" t="n">
         <v>2.0869565217391304</v>
@@ -10663,7 +11311,7 @@
         <v>330</v>
       </c>
       <c r="C72" t="s">
-        <v>330</v>
+        <v>546</v>
       </c>
       <c r="D72" t="n">
         <v>0.8947368421052632</v>
@@ -10687,7 +11335,7 @@
         <v>0.42480634229000236</v>
       </c>
       <c r="K72" t="n">
-        <v>0.6736031738775599</v>
+        <v>0.6736031738775605</v>
       </c>
       <c r="L72" t="n">
         <v>3.1956521739130435</v>
@@ -10792,7 +11440,7 @@
         <v>331</v>
       </c>
       <c r="C73" t="s">
-        <v>331</v>
+        <v>547</v>
       </c>
       <c r="D73" t="n">
         <v>-0.2857142857142857</v>
@@ -10921,7 +11569,7 @@
         <v>332</v>
       </c>
       <c r="C74" t="s">
-        <v>332</v>
+        <v>548</v>
       </c>
       <c r="D74" t="n">
         <v>0.125</v>
@@ -10945,7 +11593,7 @@
         <v>0.5453968253968254</v>
       </c>
       <c r="K74" t="n">
-        <v>0.7200562487191551</v>
+        <v>0.7200562487191552</v>
       </c>
       <c r="L74" t="n">
         <v>3.5254237288135593</v>
@@ -11050,7 +11698,7 @@
         <v>333</v>
       </c>
       <c r="C75" t="s">
-        <v>333</v>
+        <v>549</v>
       </c>
       <c r="D75" t="n">
         <v>-0.15384615384615385</v>
@@ -11074,7 +11722,7 @@
         <v>0.5151515151515151</v>
       </c>
       <c r="K75" t="n">
-        <v>0.7204348544233157</v>
+        <v>0.7204348544233163</v>
       </c>
       <c r="L75" t="n">
         <v>3.217391304347826</v>
@@ -11179,7 +11827,7 @@
         <v>334</v>
       </c>
       <c r="C76" t="s">
-        <v>334</v>
+        <v>550</v>
       </c>
       <c r="D76" t="n">
         <v>0.0</v>
@@ -11203,7 +11851,7 @@
         <v>0.5578703703703702</v>
       </c>
       <c r="K76" t="n">
-        <v>0.5376470418813523</v>
+        <v>0.5376470418813519</v>
       </c>
       <c r="L76" t="n">
         <v>3.5319148936170213</v>
@@ -11308,7 +11956,7 @@
         <v>335</v>
       </c>
       <c r="C77" t="s">
-        <v>335</v>
+        <v>551</v>
       </c>
       <c r="D77" t="n">
         <v>-0.25</v>
@@ -11332,7 +11980,7 @@
         <v>0.5950413223140496</v>
       </c>
       <c r="K77" t="n">
-        <v>0.7636558774525602</v>
+        <v>0.7636558774525605</v>
       </c>
       <c r="L77" t="n">
         <v>3.5384615384615383</v>
@@ -11437,7 +12085,7 @@
         <v>336</v>
       </c>
       <c r="C78" t="s">
-        <v>336</v>
+        <v>552</v>
       </c>
       <c r="D78" t="n">
         <v>0.4583333333333333</v>
@@ -11461,7 +12109,7 @@
         <v>0.6030245746691871</v>
       </c>
       <c r="K78" t="n">
-        <v>0.7255496218640082</v>
+        <v>0.725549621864008</v>
       </c>
       <c r="L78" t="n">
         <v>2.365079365079365</v>
@@ -11566,7 +12214,7 @@
         <v>337</v>
       </c>
       <c r="C79" t="s">
-        <v>337</v>
+        <v>553</v>
       </c>
       <c r="D79" t="n">
         <v>0.2222222222222222</v>
@@ -11590,7 +12238,7 @@
         <v>0.5743944636678201</v>
       </c>
       <c r="K79" t="n">
-        <v>0.6684707170940083</v>
+        <v>0.6684707170940085</v>
       </c>
       <c r="L79" t="n">
         <v>1.7142857142857142</v>
@@ -11695,7 +12343,7 @@
         <v>338</v>
       </c>
       <c r="C80" t="s">
-        <v>338</v>
+        <v>554</v>
       </c>
       <c r="D80" t="n">
         <v>-0.5</v>
@@ -11719,7 +12367,7 @@
         <v>0.540495867768595</v>
       </c>
       <c r="K80" t="n">
-        <v>0.7194489972394088</v>
+        <v>0.7194489972394086</v>
       </c>
       <c r="L80" t="n">
         <v>1.4210526315789473</v>
@@ -11824,7 +12472,7 @@
         <v>339</v>
       </c>
       <c r="C81" t="s">
-        <v>339</v>
+        <v>555</v>
       </c>
       <c r="D81" t="n">
         <v>0.10526315789473684</v>
@@ -11848,7 +12496,7 @@
         <v>0.6136528685548294</v>
       </c>
       <c r="K81" t="n">
-        <v>0.6638037066181901</v>
+        <v>0.6638037066181904</v>
       </c>
       <c r="L81" t="n">
         <v>1.4</v>
@@ -11953,7 +12601,7 @@
         <v>340</v>
       </c>
       <c r="C82" t="s">
-        <v>340</v>
+        <v>556</v>
       </c>
       <c r="D82" t="n">
         <v>0.06666666666666667</v>
@@ -11977,7 +12625,7 @@
         <v>0.6043956043956044</v>
       </c>
       <c r="K82" t="n">
-        <v>0.6192501947457054</v>
+        <v>0.6192501947457052</v>
       </c>
       <c r="L82" t="n">
         <v>1.588235294117647</v>
@@ -12082,7 +12730,7 @@
         <v>341</v>
       </c>
       <c r="C83" t="s">
-        <v>341</v>
+        <v>557</v>
       </c>
       <c r="D83" t="n">
         <v>-0.1875</v>
@@ -12106,7 +12754,7 @@
         <v>0.5466666666666666</v>
       </c>
       <c r="K83" t="n">
-        <v>0.6768721242021913</v>
+        <v>0.6768721242021917</v>
       </c>
       <c r="L83" t="n">
         <v>2.6666666666666665</v>
@@ -12211,7 +12859,7 @@
         <v>342</v>
       </c>
       <c r="C84" t="s">
-        <v>342</v>
+        <v>558</v>
       </c>
       <c r="D84" t="n">
         <v>0.5714285714285714</v>
@@ -12235,7 +12883,7 @@
         <v>0.6203155818540433</v>
       </c>
       <c r="K84" t="n">
-        <v>0.6720556872697134</v>
+        <v>0.6720556872697133</v>
       </c>
       <c r="L84" t="n">
         <v>3.4918032786885247</v>
@@ -12340,7 +12988,7 @@
         <v>343</v>
       </c>
       <c r="C85" t="s">
-        <v>343</v>
+        <v>559</v>
       </c>
       <c r="D85" t="n">
         <v>0.42857142857142855</v>
@@ -12364,7 +13012,7 @@
         <v>0.5621301775147929</v>
       </c>
       <c r="K85" t="n">
-        <v>0.611111111111111</v>
+        <v>0.6111111111111113</v>
       </c>
       <c r="L85" t="n">
         <v>1.8571428571428572</v>
@@ -12469,7 +13117,7 @@
         <v>344</v>
       </c>
       <c r="C86" t="s">
-        <v>344</v>
+        <v>560</v>
       </c>
       <c r="D86" t="n">
         <v>0.0</v>
@@ -12493,7 +13141,7 @@
         <v>0.5795454545454546</v>
       </c>
       <c r="K86" t="n">
-        <v>0.5876751203535702</v>
+        <v>0.5876751203535705</v>
       </c>
       <c r="L86" t="n">
         <v>2.8</v>
@@ -12598,7 +13246,7 @@
         <v>345</v>
       </c>
       <c r="C87" t="s">
-        <v>345</v>
+        <v>561</v>
       </c>
       <c r="D87" t="n">
         <v>-0.42857142857142855</v>
@@ -12622,7 +13270,7 @@
         <v>0.2672583826429979</v>
       </c>
       <c r="K87" t="n">
-        <v>0.46503133108276024</v>
+        <v>0.46503133108275946</v>
       </c>
       <c r="L87" t="n">
         <v>5.319587628865979</v>
@@ -12727,7 +13375,7 @@
         <v>346</v>
       </c>
       <c r="C88" t="s">
-        <v>346</v>
+        <v>562</v>
       </c>
       <c r="D88" t="n">
         <v>0.043478260869565216</v>
@@ -12856,7 +13504,7 @@
         <v>347</v>
       </c>
       <c r="C89" t="s">
-        <v>347</v>
+        <v>563</v>
       </c>
       <c r="D89" t="n">
         <v>-0.4444444444444444</v>
@@ -12880,7 +13528,7 @@
         <v>0.5177335640138409</v>
       </c>
       <c r="K89" t="n">
-        <v>0.7073807095794548</v>
+        <v>0.7073807095794546</v>
       </c>
       <c r="L89" t="n">
         <v>3.3846153846153846</v>
@@ -12985,7 +13633,7 @@
         <v>348</v>
       </c>
       <c r="C90" t="s">
-        <v>348</v>
+        <v>564</v>
       </c>
       <c r="D90" t="n">
         <v>0.0625</v>
@@ -13009,7 +13657,7 @@
         <v>0.5365079365079365</v>
       </c>
       <c r="K90" t="n">
-        <v>0.6290211899793113</v>
+        <v>0.6290211899793112</v>
       </c>
       <c r="L90" t="n">
         <v>3.5789473684210527</v>
@@ -13114,7 +13762,7 @@
         <v>349</v>
       </c>
       <c r="C91" t="s">
-        <v>349</v>
+        <v>565</v>
       </c>
       <c r="D91" t="n">
         <v>0.4</v>
@@ -13138,7 +13786,7 @@
         <v>0.6883830455259027</v>
       </c>
       <c r="K91" t="n">
-        <v>0.7670059672747958</v>
+        <v>0.7670059672747954</v>
       </c>
       <c r="L91" t="n">
         <v>1.9523809523809523</v>
@@ -13243,7 +13891,7 @@
         <v>350</v>
       </c>
       <c r="C92" t="s">
-        <v>350</v>
+        <v>566</v>
       </c>
       <c r="D92" t="n">
         <v>0.48</v>
@@ -13372,7 +14020,7 @@
         <v>351</v>
       </c>
       <c r="C93" t="s">
-        <v>351</v>
+        <v>567</v>
       </c>
       <c r="D93" t="n">
         <v>0.8235294117647058</v>
@@ -13501,7 +14149,7 @@
         <v>352</v>
       </c>
       <c r="C94" t="s">
-        <v>352</v>
+        <v>568</v>
       </c>
       <c r="D94" t="n">
         <v>0.22727272727272727</v>
@@ -13525,7 +14173,7 @@
         <v>0.6217687074829932</v>
       </c>
       <c r="K94" t="n">
-        <v>0.8011677544593899</v>
+        <v>0.8011677544593898</v>
       </c>
       <c r="L94" t="n">
         <v>3.086206896551724</v>
@@ -13630,7 +14278,7 @@
         <v>353</v>
       </c>
       <c r="C95" t="s">
-        <v>353</v>
+        <v>569</v>
       </c>
       <c r="D95" t="n">
         <v>-0.9375</v>
@@ -13654,7 +14302,7 @@
         <v>0.6753439153439154</v>
       </c>
       <c r="K95" t="n">
-        <v>0.7529364663571053</v>
+        <v>0.7529364663571052</v>
       </c>
       <c r="L95" t="n">
         <v>3.3777777777777778</v>
@@ -13759,7 +14407,7 @@
         <v>354</v>
       </c>
       <c r="C96" t="s">
-        <v>354</v>
+        <v>570</v>
       </c>
       <c r="D96" t="n">
         <v>0.125</v>
@@ -13783,7 +14431,7 @@
         <v>0.5047619047619047</v>
       </c>
       <c r="K96" t="n">
-        <v>0.6568028603790262</v>
+        <v>0.6568028603790268</v>
       </c>
       <c r="L96" t="n">
         <v>1.836734693877551</v>
@@ -13888,7 +14536,7 @@
         <v>355</v>
       </c>
       <c r="C97" t="s">
-        <v>355</v>
+        <v>571</v>
       </c>
       <c r="D97" t="n">
         <v>0.7647058823529411</v>
@@ -13912,7 +14560,7 @@
         <v>0.5575520833333333</v>
       </c>
       <c r="K97" t="n">
-        <v>0.7219433793087968</v>
+        <v>0.7219433793087969</v>
       </c>
       <c r="L97" t="n">
         <v>2.0</v>
@@ -14017,7 +14665,7 @@
         <v>356</v>
       </c>
       <c r="C98" t="s">
-        <v>356</v>
+        <v>572</v>
       </c>
       <c r="D98" t="n">
         <v>0.9333333333333333</v>
@@ -14041,7 +14689,7 @@
         <v>0.5039246467817896</v>
       </c>
       <c r="K98" t="n">
-        <v>0.7716570891890006</v>
+        <v>0.7716570891889998</v>
       </c>
       <c r="L98" t="n">
         <v>3.727272727272727</v>
@@ -14146,7 +14794,7 @@
         <v>357</v>
       </c>
       <c r="C99" t="s">
-        <v>357</v>
+        <v>573</v>
       </c>
       <c r="D99" t="n">
         <v>-0.06666666666666667</v>
@@ -14170,7 +14818,7 @@
         <v>0.5643642072213501</v>
       </c>
       <c r="K99" t="n">
-        <v>0.7658848514477259</v>
+        <v>0.7658848514477261</v>
       </c>
       <c r="L99" t="n">
         <v>1.6388888888888888</v>
@@ -14275,7 +14923,7 @@
         <v>358</v>
       </c>
       <c r="C100" t="s">
-        <v>358</v>
+        <v>574</v>
       </c>
       <c r="D100" t="n">
         <v>0.2222222222222222</v>
@@ -14299,7 +14947,7 @@
         <v>0.4679930795847751</v>
       </c>
       <c r="K100" t="n">
-        <v>0.6341900197201942</v>
+        <v>0.634190019720194</v>
       </c>
       <c r="L100" t="n">
         <v>1.631578947368421</v>
@@ -14404,7 +15052,7 @@
         <v>359</v>
       </c>
       <c r="C101" t="s">
-        <v>359</v>
+        <v>575</v>
       </c>
       <c r="D101" t="n">
         <v>0.38461538461538464</v>
@@ -14428,7 +15076,7 @@
         <v>0.6957070707070707</v>
       </c>
       <c r="K101" t="n">
-        <v>0.69522155996218</v>
+        <v>0.6952215599621803</v>
       </c>
       <c r="L101" t="n">
         <v>1.85</v>
@@ -14533,7 +15181,7 @@
         <v>360</v>
       </c>
       <c r="C102" t="s">
-        <v>360</v>
+        <v>576</v>
       </c>
       <c r="D102" t="n">
         <v>0.3076923076923077</v>
@@ -14662,7 +15310,7 @@
         <v>361</v>
       </c>
       <c r="C103" t="s">
-        <v>361</v>
+        <v>577</v>
       </c>
       <c r="D103" t="n">
         <v>0.7142857142857143</v>
@@ -14791,7 +15439,7 @@
         <v>362</v>
       </c>
       <c r="C104" t="s">
-        <v>362</v>
+        <v>578</v>
       </c>
       <c r="D104" t="n">
         <v>0.25</v>
@@ -14815,7 +15463,7 @@
         <v>0.11589402355792013</v>
       </c>
       <c r="K104" t="n">
-        <v>0.43249991370841595</v>
+        <v>0.43249991370841584</v>
       </c>
       <c r="L104" t="n">
         <v>4.375722543352601</v>
@@ -14920,7 +15568,7 @@
         <v>363</v>
       </c>
       <c r="C105" t="s">
-        <v>363</v>
+        <v>579</v>
       </c>
       <c r="D105" t="n">
         <v>0.0</v>
@@ -15047,7 +15695,7 @@
         <v>364</v>
       </c>
       <c r="C106" t="s">
-        <v>364</v>
+        <v>580</v>
       </c>
       <c r="D106" t="n">
         <v>1.0</v>
@@ -15071,7 +15719,7 @@
         <v>0.500865051903114</v>
       </c>
       <c r="K106" t="n">
-        <v>0.6543696995514876</v>
+        <v>0.6543696995514867</v>
       </c>
       <c r="L106" t="n">
         <v>2.546875</v>
@@ -15176,7 +15824,7 @@
         <v>365</v>
       </c>
       <c r="C107" t="s">
-        <v>365</v>
+        <v>581</v>
       </c>
       <c r="D107" t="n">
         <v>0.6153846153846154</v>
@@ -15200,7 +15848,7 @@
         <v>0.5321969696969697</v>
       </c>
       <c r="K107" t="n">
-        <v>0.705153276274636</v>
+        <v>0.7051532762746363</v>
       </c>
       <c r="L107" t="n">
         <v>1.6857142857142857</v>
@@ -15305,7 +15953,7 @@
         <v>366</v>
       </c>
       <c r="C108" t="s">
-        <v>366</v>
+        <v>582</v>
       </c>
       <c r="D108" t="n">
         <v>-0.05</v>
@@ -15329,7 +15977,7 @@
         <v>0.46044936903662664</v>
       </c>
       <c r="K108" t="n">
-        <v>0.7031830653922927</v>
+        <v>0.703183065392293</v>
       </c>
       <c r="L108" t="n">
         <v>4.101351351351352</v>
@@ -15434,7 +16082,7 @@
         <v>367</v>
       </c>
       <c r="C109" t="s">
-        <v>367</v>
+        <v>583</v>
       </c>
       <c r="D109" t="n">
         <v>0.4666666666666667</v>
@@ -15563,7 +16211,7 @@
         <v>368</v>
       </c>
       <c r="C110" t="s">
-        <v>368</v>
+        <v>584</v>
       </c>
       <c r="D110" t="n">
         <v>1.1333333333333333</v>
@@ -15587,7 +16235,7 @@
         <v>0.6554160125588697</v>
       </c>
       <c r="K110" t="n">
-        <v>0.7781497533091722</v>
+        <v>0.7781497533091724</v>
       </c>
       <c r="L110" t="n">
         <v>3.1346153846153846</v>
@@ -15692,7 +16340,7 @@
         <v>369</v>
       </c>
       <c r="C111" t="s">
-        <v>369</v>
+        <v>585</v>
       </c>
       <c r="D111" t="n">
         <v>-0.1111111111111111</v>
@@ -15716,7 +16364,7 @@
         <v>0.41738754325259514</v>
       </c>
       <c r="K111" t="n">
-        <v>0.5932868346495674</v>
+        <v>0.5932868346495678</v>
       </c>
       <c r="L111" t="n">
         <v>2.586206896551724</v>
@@ -15821,7 +16469,7 @@
         <v>370</v>
       </c>
       <c r="C112" t="s">
-        <v>370</v>
+        <v>586</v>
       </c>
       <c r="D112" t="n">
         <v>0.6666666666666666</v>
@@ -15845,7 +16493,7 @@
         <v>0.6214876033057851</v>
       </c>
       <c r="K112" t="n">
-        <v>0.6848446400614063</v>
+        <v>0.6848446400614068</v>
       </c>
       <c r="L112" t="n">
         <v>1.5217391304347827</v>
@@ -15950,7 +16598,7 @@
         <v>371</v>
       </c>
       <c r="C113" t="s">
-        <v>371</v>
+        <v>587</v>
       </c>
       <c r="D113" t="n">
         <v>0.9230769230769231</v>
@@ -16079,7 +16727,7 @@
         <v>372</v>
       </c>
       <c r="C114" t="s">
-        <v>372</v>
+        <v>588</v>
       </c>
       <c r="D114" t="n">
         <v>-0.2857142857142857</v>
@@ -16208,7 +16856,7 @@
         <v>373</v>
       </c>
       <c r="C115" t="s">
-        <v>373</v>
+        <v>589</v>
       </c>
       <c r="D115" t="n">
         <v>0.4</v>
@@ -16232,7 +16880,7 @@
         <v>0.6067503924646782</v>
       </c>
       <c r="K115" t="n">
-        <v>0.760562242927217</v>
+        <v>0.7605622429272167</v>
       </c>
       <c r="L115" t="n">
         <v>1.9565217391304348</v>
@@ -16337,7 +16985,7 @@
         <v>374</v>
       </c>
       <c r="C116" t="s">
-        <v>374</v>
+        <v>590</v>
       </c>
       <c r="D116" t="n">
         <v>0.3333333333333333</v>
@@ -16361,7 +17009,7 @@
         <v>0.7095761381475667</v>
       </c>
       <c r="K116" t="n">
-        <v>0.6406033454421222</v>
+        <v>0.640603345442122</v>
       </c>
       <c r="L116" t="n">
         <v>2.4693877551020407</v>
@@ -16466,7 +17114,7 @@
         <v>375</v>
       </c>
       <c r="C117" t="s">
-        <v>375</v>
+        <v>591</v>
       </c>
       <c r="D117" t="n">
         <v>-0.25</v>
@@ -16490,7 +17138,7 @@
         <v>0.47107438016528924</v>
       </c>
       <c r="K117" t="n">
-        <v>0.5522465746544817</v>
+        <v>0.5522465746544815</v>
       </c>
       <c r="L117" t="n">
         <v>1.5</v>
@@ -16595,7 +17243,7 @@
         <v>376</v>
       </c>
       <c r="C118" t="s">
-        <v>376</v>
+        <v>592</v>
       </c>
       <c r="D118" t="n">
         <v>0.5714285714285714</v>
@@ -16619,7 +17267,7 @@
         <v>0.4832347140039448</v>
       </c>
       <c r="K118" t="n">
-        <v>0.7323990412506672</v>
+        <v>0.7323990412506669</v>
       </c>
       <c r="L118" t="n">
         <v>2.4464285714285716</v>
@@ -16724,7 +17372,7 @@
         <v>377</v>
       </c>
       <c r="C119" t="s">
-        <v>377</v>
+        <v>593</v>
       </c>
       <c r="D119" t="n">
         <v>0.13333333333333333</v>
@@ -16748,7 +17396,7 @@
         <v>0.6883830455259027</v>
       </c>
       <c r="K119" t="n">
-        <v>0.7670059672747954</v>
+        <v>0.7670059672747956</v>
       </c>
       <c r="L119" t="n">
         <v>2.289473684210526</v>
@@ -16853,7 +17501,7 @@
         <v>378</v>
       </c>
       <c r="C120" t="s">
-        <v>378</v>
+        <v>594</v>
       </c>
       <c r="D120" t="n">
         <v>-0.2857142857142857</v>
@@ -16982,7 +17630,7 @@
         <v>379</v>
       </c>
       <c r="C121" t="s">
-        <v>379</v>
+        <v>595</v>
       </c>
       <c r="D121" t="n">
         <v>0.2777777777777778</v>
@@ -17111,7 +17759,7 @@
         <v>380</v>
       </c>
       <c r="C122" t="s">
-        <v>380</v>
+        <v>596</v>
       </c>
       <c r="D122" t="n">
         <v>0.13333333333333333</v>
@@ -17135,7 +17783,7 @@
         <v>0.6125360964837778</v>
       </c>
       <c r="K122" t="n">
-        <v>0.8149605674668173</v>
+        <v>0.8149605674668184</v>
       </c>
       <c r="L122" t="n">
         <v>2.1192660550458715</v>
@@ -17240,7 +17888,7 @@
         <v>381</v>
       </c>
       <c r="C123" t="s">
-        <v>381</v>
+        <v>597</v>
       </c>
       <c r="D123" t="n">
         <v>0.17647058823529413</v>
@@ -17264,7 +17912,7 @@
         <v>0.5255208333333333</v>
       </c>
       <c r="K123" t="n">
-        <v>0.6775443814180124</v>
+        <v>0.6775443814180122</v>
       </c>
       <c r="L123" t="n">
         <v>2.051282051282051</v>
@@ -17369,7 +18017,7 @@
         <v>382</v>
       </c>
       <c r="C124" t="s">
-        <v>382</v>
+        <v>598</v>
       </c>
       <c r="D124" t="n">
         <v>-0.05263157894736842</v>
@@ -17393,7 +18041,7 @@
         <v>0.6372549019607843</v>
       </c>
       <c r="K124" t="n">
-        <v>0.6651706006880541</v>
+        <v>0.6651706006880543</v>
       </c>
       <c r="L124" t="n">
         <v>1.6666666666666667</v>
@@ -17498,7 +18146,7 @@
         <v>383</v>
       </c>
       <c r="C125" t="s">
-        <v>383</v>
+        <v>599</v>
       </c>
       <c r="D125" t="n">
         <v>0.8333333333333334</v>
@@ -17522,7 +18170,7 @@
         <v>0.41983471074380163</v>
       </c>
       <c r="K125" t="n">
-        <v>0.5471466884461422</v>
+        <v>0.5471466884461431</v>
       </c>
       <c r="L125" t="n">
         <v>2.6551724137931036</v>
@@ -17627,7 +18275,7 @@
         <v>384</v>
       </c>
       <c r="C126" t="s">
-        <v>384</v>
+        <v>600</v>
       </c>
       <c r="D126" t="n">
         <v>-0.21428571428571427</v>
@@ -17651,7 +18299,7 @@
         <v>0.5374753451676528</v>
       </c>
       <c r="K126" t="n">
-        <v>0.655326840423217</v>
+        <v>0.6553268404232157</v>
       </c>
       <c r="L126" t="n">
         <v>1.7954545454545454</v>
@@ -17756,7 +18404,7 @@
         <v>385</v>
       </c>
       <c r="C127" t="s">
-        <v>385</v>
+        <v>601</v>
       </c>
       <c r="D127" t="n">
         <v>-0.17647058823529413</v>
@@ -17780,7 +18428,7 @@
         <v>0.4006076388888889</v>
       </c>
       <c r="K127" t="n">
-        <v>0.5352996816101623</v>
+        <v>0.5352996816101626</v>
       </c>
       <c r="L127" t="n">
         <v>1.9622641509433962</v>
@@ -17885,7 +18533,7 @@
         <v>386</v>
       </c>
       <c r="C128" t="s">
-        <v>386</v>
+        <v>602</v>
       </c>
       <c r="D128" t="n">
         <v>-0.09090909090909091</v>
@@ -17909,7 +18557,7 @@
         <v>0.5670445956160242</v>
       </c>
       <c r="K128" t="n">
-        <v>0.7520380747830183</v>
+        <v>0.7520380747830199</v>
       </c>
       <c r="L128" t="n">
         <v>2.8666666666666667</v>
@@ -18014,7 +18662,7 @@
         <v>387</v>
       </c>
       <c r="C129" t="s">
-        <v>387</v>
+        <v>603</v>
       </c>
       <c r="D129" t="n">
         <v>0.375</v>
@@ -18038,7 +18686,7 @@
         <v>0.7276190476190476</v>
       </c>
       <c r="K129" t="n">
-        <v>0.7964880732177572</v>
+        <v>0.796488073217757</v>
       </c>
       <c r="L129" t="n">
         <v>1.6590909090909092</v>
@@ -18143,7 +18791,7 @@
         <v>388</v>
       </c>
       <c r="C130" t="s">
-        <v>388</v>
+        <v>604</v>
       </c>
       <c r="D130" t="n">
         <v>0.8461538461538461</v>
@@ -18167,7 +18815,7 @@
         <v>0.25570586820586816</v>
       </c>
       <c r="K130" t="n">
-        <v>0.33376748287515895</v>
+        <v>0.3337674828751594</v>
       </c>
       <c r="L130" t="n">
         <v>3.0357142857142856</v>
@@ -18272,7 +18920,7 @@
         <v>389</v>
       </c>
       <c r="C131" t="s">
-        <v>389</v>
+        <v>605</v>
       </c>
       <c r="D131" t="n">
         <v>1.0</v>
@@ -18401,7 +19049,7 @@
         <v>390</v>
       </c>
       <c r="C132" t="s">
-        <v>390</v>
+        <v>606</v>
       </c>
       <c r="D132" t="n">
         <v>0.36363636363636365</v>
@@ -18530,7 +19178,7 @@
         <v>391</v>
       </c>
       <c r="C133" t="s">
-        <v>391</v>
+        <v>607</v>
       </c>
       <c r="D133" t="n">
         <v>1.2666666666666666</v>
@@ -18554,7 +19202,7 @@
         <v>0.5096153846153846</v>
       </c>
       <c r="K133" t="n">
-        <v>0.6908948344366228</v>
+        <v>0.6908948344366225</v>
       </c>
       <c r="L133" t="n">
         <v>1.625</v>
@@ -18659,7 +19307,7 @@
         <v>392</v>
       </c>
       <c r="C134" t="s">
-        <v>392</v>
+        <v>608</v>
       </c>
       <c r="D134" t="n">
         <v>0.058823529411764705</v>
@@ -18788,7 +19436,7 @@
         <v>393</v>
       </c>
       <c r="C135" t="s">
-        <v>393</v>
+        <v>609</v>
       </c>
       <c r="D135" t="n">
         <v>0.8888888888888888</v>
@@ -18917,7 +19565,7 @@
         <v>394</v>
       </c>
       <c r="C136" t="s">
-        <v>394</v>
+        <v>610</v>
       </c>
       <c r="D136" t="n">
         <v>0.9285714285714286</v>
@@ -18941,7 +19589,7 @@
         <v>0.616370808678501</v>
       </c>
       <c r="K136" t="n">
-        <v>0.7280452596986561</v>
+        <v>0.7280452596986553</v>
       </c>
       <c r="L136" t="n">
         <v>1.5454545454545454</v>
@@ -19046,7 +19694,7 @@
         <v>395</v>
       </c>
       <c r="C137" t="s">
-        <v>395</v>
+        <v>611</v>
       </c>
       <c r="D137" t="n">
         <v>-0.2727272727272727</v>
@@ -19070,7 +19718,7 @@
         <v>0.5925925925925926</v>
       </c>
       <c r="K137" t="n">
-        <v>0.5242080512939443</v>
+        <v>0.5242080512939442</v>
       </c>
       <c r="L137" t="n">
         <v>2.4074074074074074</v>
@@ -19175,7 +19823,7 @@
         <v>396</v>
       </c>
       <c r="C138" t="s">
-        <v>396</v>
+        <v>612</v>
       </c>
       <c r="D138" t="n">
         <v>0.09090909090909091</v>
@@ -19304,7 +19952,7 @@
         <v>397</v>
       </c>
       <c r="C139" t="s">
-        <v>397</v>
+        <v>613</v>
       </c>
       <c r="D139" t="n">
         <v>0.21052631578947367</v>
@@ -19328,7 +19976,7 @@
         <v>0.6009440813362382</v>
       </c>
       <c r="K139" t="n">
-        <v>0.6389302142172324</v>
+        <v>0.6389302142172326</v>
       </c>
       <c r="L139" t="n">
         <v>2.9714285714285715</v>
@@ -19433,7 +20081,7 @@
         <v>398</v>
       </c>
       <c r="C140" t="s">
-        <v>398</v>
+        <v>614</v>
       </c>
       <c r="D140" t="n">
         <v>0.23076923076923078</v>
@@ -19457,7 +20105,7 @@
         <v>0.4217171717171717</v>
       </c>
       <c r="K140" t="n">
-        <v>0.6031244934979115</v>
+        <v>0.603124493497912</v>
       </c>
       <c r="L140" t="n">
         <v>2.1714285714285713</v>
@@ -19562,7 +20210,7 @@
         <v>399</v>
       </c>
       <c r="C141" t="s">
-        <v>399</v>
+        <v>615</v>
       </c>
       <c r="D141" t="n">
         <v>0.631578947368421</v>
@@ -19586,7 +20234,7 @@
         <v>0.6216412490922295</v>
       </c>
       <c r="K141" t="n">
-        <v>0.6548896519663273</v>
+        <v>0.6548896519663272</v>
       </c>
       <c r="L141" t="n">
         <v>5.052083333333333</v>
@@ -19691,7 +20339,7 @@
         <v>400</v>
       </c>
       <c r="C142" t="s">
-        <v>400</v>
+        <v>616</v>
       </c>
       <c r="D142" t="n">
         <v>0.05555555555555555</v>
@@ -19715,7 +20363,7 @@
         <v>0.620242214532872</v>
       </c>
       <c r="K142" t="n">
-        <v>0.683926802509633</v>
+        <v>0.6839268025096327</v>
       </c>
       <c r="L142" t="n">
         <v>1.4482758620689655</v>
@@ -19820,7 +20468,7 @@
         <v>401</v>
       </c>
       <c r="C143" t="s">
-        <v>401</v>
+        <v>617</v>
       </c>
       <c r="D143" t="n">
         <v>0.6</v>
@@ -19844,7 +20492,7 @@
         <v>0.6185243328100472</v>
       </c>
       <c r="K143" t="n">
-        <v>0.6780697258712607</v>
+        <v>0.6780697258712605</v>
       </c>
       <c r="L143" t="n">
         <v>2.25531914893617</v>
@@ -19949,7 +20597,7 @@
         <v>402</v>
       </c>
       <c r="C144" t="s">
-        <v>402</v>
+        <v>618</v>
       </c>
       <c r="D144" t="n">
         <v>0.3125</v>
@@ -19973,7 +20621,7 @@
         <v>0.5644444444444444</v>
       </c>
       <c r="K144" t="n">
-        <v>0.7435764189605305</v>
+        <v>0.743576418960531</v>
       </c>
       <c r="L144" t="n">
         <v>2.217391304347826</v>
@@ -20078,7 +20726,7 @@
         <v>403</v>
       </c>
       <c r="C145" t="s">
-        <v>403</v>
+        <v>619</v>
       </c>
       <c r="D145" t="n">
         <v>1.3846153846153846</v>
@@ -20102,7 +20750,7 @@
         <v>1.0</v>
       </c>
       <c r="K145" t="n">
-        <v>0.775990762260204</v>
+        <v>0.7759907622602042</v>
       </c>
       <c r="L145" t="n">
         <v>2.71875</v>
@@ -20203,7 +20851,7 @@
         <v>404</v>
       </c>
       <c r="C146" t="s">
-        <v>404</v>
+        <v>620</v>
       </c>
       <c r="D146" t="n">
         <v>-0.43333333333333335</v>
@@ -20227,7 +20875,7 @@
         <v>0.5621708850008494</v>
       </c>
       <c r="K146" t="n">
-        <v>0.7230622796066134</v>
+        <v>0.723062279606614</v>
       </c>
       <c r="L146" t="n">
         <v>4.60655737704918</v>
@@ -20332,7 +20980,7 @@
         <v>405</v>
       </c>
       <c r="C147" t="s">
-        <v>405</v>
+        <v>621</v>
       </c>
       <c r="D147" t="n">
         <v>0.0</v>
@@ -20461,7 +21109,7 @@
         <v>406</v>
       </c>
       <c r="C148" t="s">
-        <v>406</v>
+        <v>622</v>
       </c>
       <c r="D148" t="n">
         <v>0.1111111111111111</v>
@@ -20485,7 +21133,7 @@
         <v>0.5051903114186851</v>
       </c>
       <c r="K148" t="n">
-        <v>0.4687389409887648</v>
+        <v>0.46873894098876523</v>
       </c>
       <c r="L148" t="n">
         <v>3.2363636363636363</v>
@@ -20590,7 +21238,7 @@
         <v>407</v>
       </c>
       <c r="C149" t="s">
-        <v>407</v>
+        <v>623</v>
       </c>
       <c r="D149" t="n">
         <v>-0.08333333333333333</v>
@@ -20614,7 +21262,7 @@
         <v>0.4677685950413223</v>
       </c>
       <c r="K149" t="n">
-        <v>0.6363346460488315</v>
+        <v>0.6363346460488312</v>
       </c>
       <c r="L149" t="n">
         <v>1.7058823529411764</v>
@@ -20719,7 +21367,7 @@
         <v>408</v>
       </c>
       <c r="C150" t="s">
-        <v>408</v>
+        <v>624</v>
       </c>
       <c r="D150" t="n">
         <v>-0.2222222222222222</v>
@@ -20743,7 +21391,7 @@
         <v>0.6254325259515571</v>
       </c>
       <c r="K150" t="n">
-        <v>0.816710751557393</v>
+        <v>0.8167107515573924</v>
       </c>
       <c r="L150" t="n">
         <v>2.119047619047619</v>
@@ -20848,7 +21496,7 @@
         <v>409</v>
       </c>
       <c r="C151" t="s">
-        <v>409</v>
+        <v>625</v>
       </c>
       <c r="D151" t="n">
         <v>-0.25</v>
@@ -20872,7 +21520,7 @@
         <v>0.6088888888888889</v>
       </c>
       <c r="K151" t="n">
-        <v>0.6533878071413065</v>
+        <v>0.653387807141306</v>
       </c>
       <c r="L151" t="n">
         <v>3.090909090909091</v>
@@ -20977,7 +21625,7 @@
         <v>410</v>
       </c>
       <c r="C152" t="s">
-        <v>410</v>
+        <v>626</v>
       </c>
       <c r="D152" t="n">
         <v>0.4666666666666667</v>
@@ -21001,7 +21649,7 @@
         <v>0.5753532182103611</v>
       </c>
       <c r="K152" t="n">
-        <v>0.6599824263157814</v>
+        <v>0.6599824263157813</v>
       </c>
       <c r="L152" t="n">
         <v>3.727272727272727</v>
@@ -21106,7 +21754,7 @@
         <v>411</v>
       </c>
       <c r="C153" t="s">
-        <v>411</v>
+        <v>627</v>
       </c>
       <c r="D153" t="n">
         <v>0.0</v>
@@ -21130,7 +21778,7 @@
         <v>0.8177777777777778</v>
       </c>
       <c r="K153" t="n">
-        <v>0.6766248927741224</v>
+        <v>0.6766248927741227</v>
       </c>
       <c r="L153" t="n">
         <v>1.8085106382978724</v>
@@ -21231,7 +21879,7 @@
         <v>412</v>
       </c>
       <c r="C154" t="s">
-        <v>412</v>
+        <v>628</v>
       </c>
       <c r="D154" t="n">
         <v>0.0</v>
@@ -21255,7 +21903,7 @@
         <v>0.6351084812623274</v>
       </c>
       <c r="K154" t="n">
-        <v>0.6921410326398418</v>
+        <v>0.6921410326398417</v>
       </c>
       <c r="L154" t="n">
         <v>3.7857142857142856</v>
@@ -21358,7 +22006,7 @@
         <v>413</v>
       </c>
       <c r="C155" t="s">
-        <v>413</v>
+        <v>629</v>
       </c>
       <c r="D155" t="n">
         <v>0.6923076923076923</v>
@@ -21382,7 +22030,7 @@
         <v>0.7209595959595959</v>
       </c>
       <c r="K155" t="n">
-        <v>0.7539578260896125</v>
+        <v>0.7539578260896126</v>
       </c>
       <c r="L155" t="n">
         <v>2.375</v>
@@ -21487,7 +22135,7 @@
         <v>414</v>
       </c>
       <c r="C156" t="s">
-        <v>414</v>
+        <v>630</v>
       </c>
       <c r="D156" t="n">
         <v>0.14285714285714285</v>
@@ -21511,7 +22159,7 @@
         <v>0.5453648915187377</v>
       </c>
       <c r="K156" t="n">
-        <v>0.572994449954603</v>
+        <v>0.5729944499546029</v>
       </c>
       <c r="L156" t="n">
         <v>2.28125</v>
@@ -21616,7 +22264,7 @@
         <v>415</v>
       </c>
       <c r="C157" t="s">
-        <v>415</v>
+        <v>631</v>
       </c>
       <c r="D157" t="n">
         <v>0.23076923076923078</v>
@@ -21640,7 +22288,7 @@
         <v>0.5820707070707071</v>
       </c>
       <c r="K157" t="n">
-        <v>0.6749707165392148</v>
+        <v>0.6749707165392153</v>
       </c>
       <c r="L157" t="n">
         <v>2.269230769230769</v>
@@ -21745,7 +22393,7 @@
         <v>416</v>
       </c>
       <c r="C158" t="s">
-        <v>416</v>
+        <v>632</v>
       </c>
       <c r="D158" t="n">
         <v>0.35714285714285715</v>
@@ -21769,7 +22417,7 @@
         <v>0.5877712031558185</v>
       </c>
       <c r="K158" t="n">
-        <v>0.6552051453440119</v>
+        <v>0.655205145344012</v>
       </c>
       <c r="L158" t="n">
         <v>3.8541666666666665</v>
@@ -21874,7 +22522,7 @@
         <v>417</v>
       </c>
       <c r="C159" t="s">
-        <v>417</v>
+        <v>633</v>
       </c>
       <c r="D159" t="n">
         <v>1.2941176470588236</v>
@@ -21898,7 +22546,7 @@
         <v>0.33671875</v>
       </c>
       <c r="K159" t="n">
-        <v>0.5560727419843986</v>
+        <v>0.5560727419843988</v>
       </c>
       <c r="L159" t="n">
         <v>1.9056603773584906</v>
@@ -22003,7 +22651,7 @@
         <v>418</v>
       </c>
       <c r="C160" t="s">
-        <v>418</v>
+        <v>634</v>
       </c>
       <c r="D160" t="n">
         <v>0.4666666666666667</v>
@@ -22027,7 +22675,7 @@
         <v>0.6043956043956044</v>
       </c>
       <c r="K160" t="n">
-        <v>0.6192501947457051</v>
+        <v>0.6192501947457052</v>
       </c>
       <c r="L160" t="n">
         <v>1.4615384615384615</v>
@@ -22132,7 +22780,7 @@
         <v>419</v>
       </c>
       <c r="C161" t="s">
-        <v>419</v>
+        <v>635</v>
       </c>
       <c r="D161" t="n">
         <v>0.14285714285714285</v>
@@ -22261,7 +22909,7 @@
         <v>420</v>
       </c>
       <c r="C162" t="s">
-        <v>420</v>
+        <v>636</v>
       </c>
       <c r="D162" t="n">
         <v>0.75</v>
@@ -22285,7 +22933,7 @@
         <v>0.39173553719008264</v>
       </c>
       <c r="K162" t="n">
-        <v>0.6383479422507059</v>
+        <v>0.6383479422507055</v>
       </c>
       <c r="L162" t="n">
         <v>2.933333333333333</v>
@@ -22390,7 +23038,7 @@
         <v>421</v>
       </c>
       <c r="C163" t="s">
-        <v>421</v>
+        <v>637</v>
       </c>
       <c r="D163" t="n">
         <v>0.0</v>
@@ -22414,7 +23062,7 @@
         <v>0.6125</v>
       </c>
       <c r="K163" t="n">
-        <v>0.6382203233266482</v>
+        <v>0.6382203233266485</v>
       </c>
       <c r="L163" t="n">
         <v>1.746031746031746</v>
@@ -22519,7 +23167,7 @@
         <v>422</v>
       </c>
       <c r="C164" t="s">
-        <v>422</v>
+        <v>638</v>
       </c>
       <c r="D164" t="n">
         <v>0.07142857142857142</v>
@@ -22543,7 +23191,7 @@
         <v>0.28479709473694903</v>
       </c>
       <c r="K164" t="n">
-        <v>0.605553099118553</v>
+        <v>0.6055530991185532</v>
       </c>
       <c r="L164" t="n">
         <v>4.278884462151394</v>
@@ -22648,7 +23296,7 @@
         <v>423</v>
       </c>
       <c r="C165" t="s">
-        <v>423</v>
+        <v>639</v>
       </c>
       <c r="D165" t="n">
         <v>0.15384615384615385</v>
@@ -22672,7 +23320,7 @@
         <v>0.6805555555555556</v>
       </c>
       <c r="K165" t="n">
-        <v>0.7503994041344021</v>
+        <v>0.7503994041344022</v>
       </c>
       <c r="L165" t="n">
         <v>1.5714285714285714</v>
@@ -22777,7 +23425,7 @@
         <v>424</v>
       </c>
       <c r="C166" t="s">
-        <v>424</v>
+        <v>640</v>
       </c>
       <c r="D166" t="n">
         <v>-0.15384615384615385</v>
@@ -22801,7 +23449,7 @@
         <v>0.5694444444444444</v>
       </c>
       <c r="K166" t="n">
-        <v>0.7295283117584025</v>
+        <v>0.7295283117584016</v>
       </c>
       <c r="L166" t="n">
         <v>1.8636363636363635</v>
@@ -22906,7 +23554,7 @@
         <v>425</v>
       </c>
       <c r="C167" t="s">
-        <v>425</v>
+        <v>641</v>
       </c>
       <c r="D167" t="n">
         <v>-0.5454545454545454</v>
@@ -22930,7 +23578,7 @@
         <v>0.44666666666666666</v>
       </c>
       <c r="K167" t="n">
-        <v>0.5138798723099929</v>
+        <v>0.5138798723099931</v>
       </c>
       <c r="L167" t="n">
         <v>1.72</v>
@@ -23035,7 +23683,7 @@
         <v>426</v>
       </c>
       <c r="C168" t="s">
-        <v>426</v>
+        <v>642</v>
       </c>
       <c r="D168" t="n">
         <v>0.42857142857142855</v>
@@ -23059,7 +23707,7 @@
         <v>0.46745562130177515</v>
       </c>
       <c r="K168" t="n">
-        <v>0.5914481721951658</v>
+        <v>0.5914481721951657</v>
       </c>
       <c r="L168" t="n">
         <v>3.150943396226415</v>
@@ -23164,7 +23812,7 @@
         <v>427</v>
       </c>
       <c r="C169" t="s">
-        <v>427</v>
+        <v>643</v>
       </c>
       <c r="D169" t="n">
         <v>0.26666666666666666</v>
@@ -23293,7 +23941,7 @@
         <v>428</v>
       </c>
       <c r="C170" t="s">
-        <v>428</v>
+        <v>644</v>
       </c>
       <c r="D170" t="n">
         <v>0.5</v>
@@ -23317,7 +23965,7 @@
         <v>0.40927021696252464</v>
       </c>
       <c r="K170" t="n">
-        <v>0.5555541941161156</v>
+        <v>0.5555541941161155</v>
       </c>
       <c r="L170" t="n">
         <v>2.0</v>
@@ -23422,7 +24070,7 @@
         <v>429</v>
       </c>
       <c r="C171" t="s">
-        <v>429</v>
+        <v>645</v>
       </c>
       <c r="D171" t="n">
         <v>0.5</v>
@@ -23551,7 +24199,7 @@
         <v>430</v>
       </c>
       <c r="C172" t="s">
-        <v>430</v>
+        <v>646</v>
       </c>
       <c r="D172" t="n">
         <v>0.38461538461538464</v>
@@ -23575,7 +24223,7 @@
         <v>0.5808080808080808</v>
       </c>
       <c r="K172" t="n">
-        <v>0.689613932880021</v>
+        <v>0.6896139328800207</v>
       </c>
       <c r="L172" t="n">
         <v>1.0</v>
@@ -23680,7 +24328,7 @@
         <v>431</v>
       </c>
       <c r="C173" t="s">
-        <v>431</v>
+        <v>647</v>
       </c>
       <c r="D173" t="n">
         <v>0.125</v>
@@ -23704,7 +24352,7 @@
         <v>0.6076190476190476</v>
       </c>
       <c r="K173" t="n">
-        <v>0.6997447656887503</v>
+        <v>0.6997447656887485</v>
       </c>
       <c r="L173" t="n">
         <v>1.2222222222222223</v>
@@ -23809,7 +24457,7 @@
         <v>432</v>
       </c>
       <c r="C174" t="s">
-        <v>432</v>
+        <v>648</v>
       </c>
       <c r="D174" t="n">
         <v>0.0</v>
@@ -23833,7 +24481,7 @@
         <v>0.653968253968254</v>
       </c>
       <c r="K174" t="n">
-        <v>0.7273681331479634</v>
+        <v>0.7273681331479638</v>
       </c>
       <c r="L174" t="n">
         <v>3.4705882352941178</v>
@@ -23938,7 +24586,7 @@
         <v>433</v>
       </c>
       <c r="C175" t="s">
-        <v>433</v>
+        <v>649</v>
       </c>
       <c r="D175" t="n">
         <v>1.2</v>
@@ -23962,7 +24610,7 @@
         <v>0.6059654631083202</v>
       </c>
       <c r="K175" t="n">
-        <v>0.7023888300243785</v>
+        <v>0.7023888300243784</v>
       </c>
       <c r="L175" t="n">
         <v>2.6206896551724137</v>
@@ -24067,7 +24715,7 @@
         <v>434</v>
       </c>
       <c r="C176" t="s">
-        <v>434</v>
+        <v>650</v>
       </c>
       <c r="D176" t="n">
         <v>0.0</v>
@@ -24091,7 +24739,7 @@
         <v>0.5277777777777778</v>
       </c>
       <c r="K176" t="n">
-        <v>0.5497246451155328</v>
+        <v>0.5497246451155332</v>
       </c>
       <c r="L176" t="n">
         <v>1.1875</v>
@@ -24196,7 +24844,7 @@
         <v>435</v>
       </c>
       <c r="C177" t="s">
-        <v>435</v>
+        <v>651</v>
       </c>
       <c r="D177" t="n">
         <v>1.0714285714285714</v>
@@ -24325,7 +24973,7 @@
         <v>436</v>
       </c>
       <c r="C178" t="s">
-        <v>436</v>
+        <v>652</v>
       </c>
       <c r="D178" t="n">
         <v>0.23076923076923078</v>
@@ -24349,7 +24997,7 @@
         <v>0.5542929292929293</v>
       </c>
       <c r="K178" t="n">
-        <v>0.7437212953676025</v>
+        <v>0.7437212953676028</v>
       </c>
       <c r="L178" t="n">
         <v>1.8518518518518519</v>
@@ -24454,7 +25102,7 @@
         <v>437</v>
       </c>
       <c r="C179" t="s">
-        <v>437</v>
+        <v>653</v>
       </c>
       <c r="D179" t="n">
         <v>0.35714285714285715</v>
@@ -24478,7 +25126,7 @@
         <v>0.6785009861932939</v>
       </c>
       <c r="K179" t="n">
-        <v>0.7872163097076945</v>
+        <v>0.7872163097076944</v>
       </c>
       <c r="L179" t="n">
         <v>1.4782608695652173</v>
@@ -24583,7 +25231,7 @@
         <v>438</v>
       </c>
       <c r="C180" t="s">
-        <v>438</v>
+        <v>654</v>
       </c>
       <c r="D180" t="n">
         <v>0.25</v>
@@ -24607,7 +25255,7 @@
         <v>0.6033057851239669</v>
       </c>
       <c r="K180" t="n">
-        <v>0.7286742057325314</v>
+        <v>0.7286742057325313</v>
       </c>
       <c r="L180" t="n">
         <v>1.5238095238095237</v>
@@ -24712,7 +25360,7 @@
         <v>439</v>
       </c>
       <c r="C181" t="s">
-        <v>439</v>
+        <v>655</v>
       </c>
       <c r="D181" t="n">
         <v>0.29411764705882354</v>
@@ -24736,7 +25384,7 @@
         <v>0.6484375</v>
       </c>
       <c r="K181" t="n">
-        <v>0.6675960467059584</v>
+        <v>0.667596046705959</v>
       </c>
       <c r="L181" t="n">
         <v>3.5483870967741935</v>
@@ -24841,7 +25489,7 @@
         <v>440</v>
       </c>
       <c r="C182" t="s">
-        <v>440</v>
+        <v>656</v>
       </c>
       <c r="D182" t="n">
         <v>0.07692307692307693</v>
@@ -24865,7 +25513,7 @@
         <v>0.5795454545454546</v>
       </c>
       <c r="K182" t="n">
-        <v>0.5876751203535704</v>
+        <v>0.5876751203535707</v>
       </c>
       <c r="L182" t="n">
         <v>1.4</v>
@@ -24970,7 +25618,7 @@
         <v>441</v>
       </c>
       <c r="C183" t="s">
-        <v>441</v>
+        <v>657</v>
       </c>
       <c r="D183" t="n">
         <v>-0.14285714285714285</v>
@@ -24994,7 +25642,7 @@
         <v>0.6607495069033531</v>
       </c>
       <c r="K183" t="n">
-        <v>0.7107858251581546</v>
+        <v>0.7107858251581547</v>
       </c>
       <c r="L183" t="n">
         <v>1.7692307692307692</v>
@@ -25099,7 +25747,7 @@
         <v>442</v>
       </c>
       <c r="C184" t="s">
-        <v>442</v>
+        <v>658</v>
       </c>
       <c r="D184" t="n">
         <v>0.0</v>
@@ -25123,7 +25771,7 @@
         <v>0.6256354393609296</v>
       </c>
       <c r="K184" t="n">
-        <v>0.7750910953322778</v>
+        <v>0.7750910953322785</v>
       </c>
       <c r="L184" t="n">
         <v>1.8545454545454545</v>
@@ -25228,7 +25876,7 @@
         <v>443</v>
       </c>
       <c r="C185" t="s">
-        <v>443</v>
+        <v>659</v>
       </c>
       <c r="D185" t="n">
         <v>0.9230769230769231</v>
@@ -25252,7 +25900,7 @@
         <v>0.5498737373737373</v>
       </c>
       <c r="K185" t="n">
-        <v>0.5921570582603476</v>
+        <v>0.5921570582603477</v>
       </c>
       <c r="L185" t="n">
         <v>1.6153846153846154</v>
@@ -25357,7 +26005,7 @@
         <v>444</v>
       </c>
       <c r="C186" t="s">
-        <v>444</v>
+        <v>660</v>
       </c>
       <c r="D186" t="n">
         <v>0.21428571428571427</v>
@@ -25381,7 +26029,7 @@
         <v>0.6400394477317555</v>
       </c>
       <c r="K186" t="n">
-        <v>0.7085243743539134</v>
+        <v>0.7085243743539135</v>
       </c>
       <c r="L186" t="n">
         <v>2.230769230769231</v>
@@ -25486,7 +26134,7 @@
         <v>445</v>
       </c>
       <c r="C187" t="s">
-        <v>445</v>
+        <v>661</v>
       </c>
       <c r="D187" t="n">
         <v>0.3333333333333333</v>
@@ -25510,7 +26158,7 @@
         <v>0.6776859504132231</v>
       </c>
       <c r="K187" t="n">
-        <v>0.7653662811812495</v>
+        <v>0.7653662811812497</v>
       </c>
       <c r="L187" t="n">
         <v>2.125</v>
@@ -25615,7 +26263,7 @@
         <v>446</v>
       </c>
       <c r="C188" t="s">
-        <v>446</v>
+        <v>662</v>
       </c>
       <c r="D188" t="n">
         <v>0.22727272727272727</v>
@@ -25639,7 +26287,7 @@
         <v>0.41020408163265304</v>
       </c>
       <c r="K188" t="n">
-        <v>0.6511862544504639</v>
+        <v>0.651186254450461</v>
       </c>
       <c r="L188" t="n">
         <v>3.619047619047619</v>
@@ -25744,7 +26392,7 @@
         <v>447</v>
       </c>
       <c r="C189" t="s">
-        <v>447</v>
+        <v>663</v>
       </c>
       <c r="D189" t="n">
         <v>0.3333333333333333</v>
@@ -25873,7 +26521,7 @@
         <v>448</v>
       </c>
       <c r="C190" t="s">
-        <v>448</v>
+        <v>664</v>
       </c>
       <c r="D190" t="n">
         <v>0.6153846153846154</v>
@@ -25897,7 +26545,7 @@
         <v>0.48547979797979796</v>
       </c>
       <c r="K190" t="n">
-        <v>0.6210125873430765</v>
+        <v>0.6210125873430767</v>
       </c>
       <c r="L190" t="n">
         <v>3.2790697674418605</v>
@@ -26002,7 +26650,7 @@
         <v>449</v>
       </c>
       <c r="C191" t="s">
-        <v>449</v>
+        <v>665</v>
       </c>
       <c r="D191" t="n">
         <v>0.5714285714285714</v>
@@ -26026,7 +26674,7 @@
         <v>0.5887573964497042</v>
       </c>
       <c r="K191" t="n">
-        <v>0.659955705635969</v>
+        <v>0.6599557056359688</v>
       </c>
       <c r="L191" t="n">
         <v>1.6774193548387097</v>
@@ -26131,7 +26779,7 @@
         <v>450</v>
       </c>
       <c r="C192" t="s">
-        <v>450</v>
+        <v>666</v>
       </c>
       <c r="D192" t="n">
         <v>0.631578947368421</v>
@@ -26155,7 +26803,7 @@
         <v>0.7000726216412491</v>
       </c>
       <c r="K192" t="n">
-        <v>0.7917764071627926</v>
+        <v>0.7917764071627923</v>
       </c>
       <c r="L192" t="n">
         <v>2.176470588235294</v>
@@ -26260,7 +26908,7 @@
         <v>451</v>
       </c>
       <c r="C193" t="s">
-        <v>451</v>
+        <v>667</v>
       </c>
       <c r="D193" t="n">
         <v>0.0625</v>
@@ -26284,7 +26932,7 @@
         <v>0.4939682539682539</v>
       </c>
       <c r="K193" t="n">
-        <v>0.6190775915470381</v>
+        <v>0.6190775915470379</v>
       </c>
       <c r="L193" t="n">
         <v>5.948717948717949</v>
@@ -26389,7 +27037,7 @@
         <v>452</v>
       </c>
       <c r="C194" t="s">
-        <v>452</v>
+        <v>668</v>
       </c>
       <c r="D194" t="n">
         <v>0.125</v>
@@ -26413,7 +27061,7 @@
         <v>0.6457142857142857</v>
       </c>
       <c r="K194" t="n">
-        <v>0.638665427269645</v>
+        <v>0.6386654272696458</v>
       </c>
       <c r="L194" t="n">
         <v>1.9807692307692308</v>
@@ -26518,7 +27166,7 @@
         <v>453</v>
       </c>
       <c r="C195" t="s">
-        <v>453</v>
+        <v>669</v>
       </c>
       <c r="D195" t="n">
         <v>0.4666666666666667</v>
@@ -26647,7 +27295,7 @@
         <v>454</v>
       </c>
       <c r="C196" t="s">
-        <v>454</v>
+        <v>670</v>
       </c>
       <c r="D196" t="n">
         <v>-0.35714285714285715</v>
@@ -26671,7 +27319,7 @@
         <v>0.47534516765285995</v>
       </c>
       <c r="K196" t="n">
-        <v>0.5801949258430955</v>
+        <v>0.5801949258430951</v>
       </c>
       <c r="L196" t="n">
         <v>2.5</v>
@@ -26776,7 +27424,7 @@
         <v>455</v>
       </c>
       <c r="C197" t="s">
-        <v>455</v>
+        <v>671</v>
       </c>
       <c r="D197" t="n">
         <v>0.3333333333333333</v>
@@ -26800,7 +27448,7 @@
         <v>0.6264462809917355</v>
       </c>
       <c r="K197" t="n">
-        <v>0.6813106699907029</v>
+        <v>0.6813106699907031</v>
       </c>
       <c r="L197" t="n">
         <v>1.631578947368421</v>
@@ -26903,7 +27551,7 @@
         <v>456</v>
       </c>
       <c r="C198" t="s">
-        <v>456</v>
+        <v>672</v>
       </c>
       <c r="D198" t="n">
         <v>0.125</v>
@@ -26927,7 +27575,7 @@
         <v>0.5053968253968254</v>
       </c>
       <c r="K198" t="n">
-        <v>0.5950426851247094</v>
+        <v>0.5950426851247089</v>
       </c>
       <c r="L198" t="n">
         <v>1.8055555555555556</v>
@@ -27032,7 +27680,7 @@
         <v>457</v>
       </c>
       <c r="C199" t="s">
-        <v>457</v>
+        <v>673</v>
       </c>
       <c r="D199" t="n">
         <v>0.35294117647058826</v>
@@ -27056,7 +27704,7 @@
         <v>0.5703125</v>
       </c>
       <c r="K199" t="n">
-        <v>0.7124215353634711</v>
+        <v>0.712421535363471</v>
       </c>
       <c r="L199" t="n">
         <v>3.7413793103448274</v>
@@ -27161,7 +27809,7 @@
         <v>458</v>
       </c>
       <c r="C200" t="s">
-        <v>458</v>
+        <v>674</v>
       </c>
       <c r="D200" t="n">
         <v>0.9285714285714286</v>
@@ -27185,7 +27833,7 @@
         <v>0.727810650887574</v>
       </c>
       <c r="K200" t="n">
-        <v>0.7451447138637768</v>
+        <v>0.7451447138637767</v>
       </c>
       <c r="L200" t="n">
         <v>4.029411764705882</v>
@@ -27290,7 +27938,7 @@
         <v>459</v>
       </c>
       <c r="C201" t="s">
-        <v>459</v>
+        <v>675</v>
       </c>
       <c r="D201" t="n">
         <v>-0.058823529411764705</v>
@@ -27314,7 +27962,7 @@
         <v>0.6229166666666667</v>
       </c>
       <c r="K201" t="n">
-        <v>0.6444444444444447</v>
+        <v>0.6444444444444446</v>
       </c>
       <c r="L201" t="n">
         <v>2.186046511627907</v>
@@ -27419,7 +28067,7 @@
         <v>460</v>
       </c>
       <c r="C202" t="s">
-        <v>460</v>
+        <v>676</v>
       </c>
       <c r="D202" t="n">
         <v>0.2857142857142857</v>
@@ -27548,7 +28196,7 @@
         <v>461</v>
       </c>
       <c r="C203" t="s">
-        <v>461</v>
+        <v>677</v>
       </c>
       <c r="D203" t="n">
         <v>-0.125</v>
@@ -27677,7 +28325,7 @@
         <v>462</v>
       </c>
       <c r="C204" t="s">
-        <v>462</v>
+        <v>678</v>
       </c>
       <c r="D204" t="n">
         <v>0.38461538461538464</v>
@@ -27701,7 +28349,7 @@
         <v>0.5795454545454546</v>
       </c>
       <c r="K204" t="n">
-        <v>0.5876751203535702</v>
+        <v>0.5876751203535707</v>
       </c>
       <c r="L204" t="n">
         <v>1.5714285714285714</v>
@@ -27806,7 +28454,7 @@
         <v>463</v>
       </c>
       <c r="C205" t="s">
-        <v>463</v>
+        <v>679</v>
       </c>
       <c r="D205" t="n">
         <v>-0.6153846153846154</v>
@@ -27935,7 +28583,7 @@
         <v>464</v>
       </c>
       <c r="C206" t="s">
-        <v>464</v>
+        <v>680</v>
       </c>
       <c r="D206" t="n">
         <v>0.0</v>
@@ -27959,7 +28607,7 @@
         <v>0.48226643598615915</v>
       </c>
       <c r="K206" t="n">
-        <v>0.6684156331758153</v>
+        <v>0.668415633175815</v>
       </c>
       <c r="L206" t="n">
         <v>1.7272727272727273</v>
@@ -28064,7 +28712,7 @@
         <v>465</v>
       </c>
       <c r="C207" t="s">
-        <v>465</v>
+        <v>681</v>
       </c>
       <c r="D207" t="n">
         <v>-0.2</v>
@@ -28193,7 +28841,7 @@
         <v>466</v>
       </c>
       <c r="C208" t="s">
-        <v>466</v>
+        <v>682</v>
       </c>
       <c r="D208" t="n">
         <v>0.8666666666666667</v>
@@ -28217,7 +28865,7 @@
         <v>0.7256671899529042</v>
       </c>
       <c r="K208" t="n">
-        <v>0.6975176159222342</v>
+        <v>0.6975176159222338</v>
       </c>
       <c r="L208" t="n">
         <v>1.56</v>
@@ -28322,7 +28970,7 @@
         <v>467</v>
       </c>
       <c r="C209" t="s">
-        <v>467</v>
+        <v>683</v>
       </c>
       <c r="D209" t="n">
         <v>0.23529411764705882</v>
@@ -28346,7 +28994,7 @@
         <v>0.5619791666666667</v>
       </c>
       <c r="K209" t="n">
-        <v>0.6431061396231923</v>
+        <v>0.6431061396231921</v>
       </c>
       <c r="L209" t="n">
         <v>1.7714285714285714</v>
@@ -28451,7 +29099,7 @@
         <v>468</v>
       </c>
       <c r="C210" t="s">
-        <v>468</v>
+        <v>684</v>
       </c>
       <c r="D210" t="n">
         <v>0.46153846153846156</v>
@@ -28475,7 +29123,7 @@
         <v>0.37247474747474746</v>
       </c>
       <c r="K210" t="n">
-        <v>0.583906988326784</v>
+        <v>0.583906988326783</v>
       </c>
       <c r="L210" t="n">
         <v>1.7727272727272727</v>
@@ -28580,7 +29228,7 @@
         <v>469</v>
       </c>
       <c r="C211" t="s">
-        <v>469</v>
+        <v>685</v>
       </c>
       <c r="D211" t="n">
         <v>0.5714285714285714</v>
@@ -28604,7 +29252,7 @@
         <v>0.5996055226824457</v>
       </c>
       <c r="K211" t="n">
-        <v>0.6337316859671392</v>
+        <v>0.6337316859671387</v>
       </c>
       <c r="L211" t="n">
         <v>1.4166666666666667</v>
@@ -28709,7 +29357,7 @@
         <v>470</v>
       </c>
       <c r="C212" t="s">
-        <v>470</v>
+        <v>686</v>
       </c>
       <c r="D212" t="n">
         <v>0.4375</v>
@@ -28838,7 +29486,7 @@
         <v>471</v>
       </c>
       <c r="C213" t="s">
-        <v>471</v>
+        <v>687</v>
       </c>
       <c r="D213" t="n">
         <v>1.5555555555555556</v>
@@ -28967,7 +29615,7 @@
         <v>472</v>
       </c>
       <c r="C214" t="s">
-        <v>472</v>
+        <v>688</v>
       </c>
       <c r="D214" t="n">
         <v>0.75</v>
@@ -28991,7 +29639,7 @@
         <v>0.6692063492063492</v>
       </c>
       <c r="K214" t="n">
-        <v>0.7297654917292117</v>
+        <v>0.7297654917292115</v>
       </c>
       <c r="L214" t="n">
         <v>2.5238095238095237</v>
@@ -29096,7 +29744,7 @@
         <v>473</v>
       </c>
       <c r="C215" t="s">
-        <v>473</v>
+        <v>689</v>
       </c>
       <c r="D215" t="n">
         <v>0.5384615384615384</v>
@@ -29120,7 +29768,7 @@
         <v>0.6805555555555556</v>
       </c>
       <c r="K215" t="n">
-        <v>0.7503994041344021</v>
+        <v>0.7503994041344023</v>
       </c>
       <c r="L215" t="n">
         <v>2.590909090909091</v>
@@ -29225,7 +29873,7 @@
         <v>474</v>
       </c>
       <c r="C216" t="s">
-        <v>474</v>
+        <v>690</v>
       </c>
       <c r="D216" t="n">
         <v>0.0</v>
@@ -29249,7 +29897,7 @@
         <v>0.4913657770800628</v>
       </c>
       <c r="K216" t="n">
-        <v>0.6466612264356273</v>
+        <v>0.646661226435627</v>
       </c>
       <c r="L216" t="n">
         <v>1.44</v>
@@ -29354,7 +30002,7 @@
         <v>475</v>
       </c>
       <c r="C217" t="s">
-        <v>475</v>
+        <v>691</v>
       </c>
       <c r="D217" t="n">
         <v>0.5</v>
@@ -29378,7 +30026,7 @@
         <v>0.645079365079365</v>
       </c>
       <c r="K217" t="n">
-        <v>0.6766073699035824</v>
+        <v>0.6766073699035827</v>
       </c>
       <c r="L217" t="n">
         <v>4.578947368421052</v>

</xml_diff>